<commit_message>
Grandes alterações: - Arquivo 'analise.ipynb' criado. - Correção: O nome do arquivo 'scrapingPcGamer' teve seu nome trocado. - Arquivo tratamento teve comentários adicionados, além de novas colunas (df['Marca'], df['Categoria']). Formatação com title case nas colunas. Coluna 'Resumo_Nome' criada para simplificar a visualização do gráfico 3.
</commit_message>
<xml_diff>
--- a/web_scraping/site_dinamico2/perifericos.xlsx
+++ b/web_scraping/site_dinamico2/perifericos.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D131"/>
+  <dimension ref="A1:E133"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -454,6 +454,11 @@
           <t>Frete</t>
         </is>
       </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>Desconto</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
@@ -475,7 +480,12 @@
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>pago</t>
+          <t>Pago</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>-9%</t>
         </is>
       </c>
     </row>
@@ -499,7 +509,12 @@
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>pago</t>
+          <t>Pago</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>0%</t>
         </is>
       </c>
     </row>
@@ -523,175 +538,215 @@
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>pago</t>
+          <t>Grátis</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>-13%</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Webcam Full HD Logitech C920s com Microfone Embutido, Proteção de Privacidade, Widescreen 1080p, Compatível Logitech Capture - 960-001257</t>
+          <t>Mouse HP 150, 1600 DPI, Dongle USB-A, Preto - 240J6AA</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>R$ 409,99</t>
+          <t>R$ 25,99</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
           <t>À vista no PIX
 ou até
-10x de R$ 46,59</t>
+1x de R$ 25,99</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>grátis</t>
+          <t>Pago</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>-13%</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>Teclado e Mouse Sem Fio Dell KM3322W, USB, ABNT2, Preto - 580-BBBB</t>
+          <t>Webcam Full HD Logitech C920s com Microfone Embutido, Proteção de Privacidade, Widescreen 1080p, Compatível Logitech Capture - 960-001257</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>R$ 159,99</t>
+          <t>R$ 409,99</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
           <t>À vista no PIX
 ou até
-7x de R$ 26,88</t>
+10x de R$ 46,59</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>pago</t>
+          <t>Grátis</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>-10%</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>Mouse com fio USB Logitech M90 com Design Ambidestro e Facilidade Plug and Play - 910-004053</t>
+          <t>Teclado e Mouse Sem Fio Dell KM3322W, USB, ABNT2, Preto - 580-BBBB</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>R$ 33,90</t>
+          <t>R$ 139,90</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
           <t>À vista no PIX
 ou até
-1x de R$ 33,90</t>
+6x de R$ 27,43</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>pago</t>
+          <t>Pago</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>-12%</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>Combo Teclado e Mouse sem fio Logitech MK220 com Design Compacto, Conexão USB, Pilhas Inclusas e Layout ABNT2 - 920-004431</t>
+          <t>Mouse com fio USB Logitech M90 com Design Ambidestro e Facilidade Plug and Play - 910-004053</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>R$ 119,99</t>
+          <t>R$ 33,90</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
           <t>À vista no PIX
 ou até
-5x de R$ 27,27</t>
+1x de R$ 33,90</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>pago</t>
+          <t>Pago</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>-15%</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>Mouse sem fio Logitech M170 com Design Ambidestro Compacto, Conexão USB e Pilha Inclusa, Preto - 910-004940</t>
+          <t>Combo Teclado e Mouse sem fio Logitech MK220 com Design Compacto, Conexão USB, Pilhas Inclusas e Layout ABNT2 - 920-004431</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>R$ 54,99</t>
+          <t>R$ 119,99</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
           <t>À vista no PIX
 ou até
-2x de R$ 28,94</t>
+5x de R$ 27,27</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>grátis</t>
+          <t>Pago</t>
+        </is>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>-14%</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>Combo Teclado e Mouse sem fio Logitech MK235 com Conexão USB, Pilhas Inclusas e Layout ABNT2 - 920-007903</t>
+          <t>Mouse sem fio Logitech M170 com Design Ambidestro Compacto, Conexão USB e Pilha Inclusa, Preto - 910-004940</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>R$ 135,90</t>
+          <t>R$ 54,99</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
           <t>À vista no PIX
 ou até
-6x de R$ 26,64</t>
+2x de R$ 28,94</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>grátis</t>
+          <t>Pago</t>
+        </is>
+      </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>-21%</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>Headset HP DHH-1601, Drivers 40mm, Conector P2 2x 3,5mm, Cabo 2m, Preto - 194S3AA</t>
+          <t>Combo Teclado e Mouse sem fio Logitech MK235 com Conexão USB, Pilhas Inclusas e Layout ABNT2 - 920-007903</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>R$ 69,90</t>
+          <t>R$ 135,90</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
           <t>À vista no PIX
 ou até
-3x de R$ 26,47</t>
+6x de R$ 26,64</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>pago</t>
+          <t>Grátis</t>
+        </is>
+      </c>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>-15%</t>
         </is>
       </c>
     </row>
@@ -703,19 +758,24 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>R$ 186,90</t>
+          <t>R$ 181,99</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
           <t>À vista no PIX
 ou até
-8x de R$ 27,48</t>
+8x de R$ 26,76</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>pago</t>
+          <t>Grátis</t>
+        </is>
+      </c>
+      <c r="E12" t="inlineStr">
+        <is>
+          <t>-17%</t>
         </is>
       </c>
     </row>
@@ -739,7 +799,12 @@
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>pago</t>
+          <t>Grátis</t>
+        </is>
+      </c>
+      <c r="E13" t="inlineStr">
+        <is>
+          <t>-17%</t>
         </is>
       </c>
     </row>
@@ -763,7 +828,12 @@
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>pago</t>
+          <t>Pago</t>
+        </is>
+      </c>
+      <c r="E14" t="inlineStr">
+        <is>
+          <t>0%</t>
         </is>
       </c>
     </row>
@@ -787,7 +857,12 @@
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>pago</t>
+          <t>Pago</t>
+        </is>
+      </c>
+      <c r="E15" t="inlineStr">
+        <is>
+          <t>-46%</t>
         </is>
       </c>
     </row>
@@ -811,7 +886,12 @@
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>pago</t>
+          <t>Pago</t>
+        </is>
+      </c>
+      <c r="E16" t="inlineStr">
+        <is>
+          <t>-18%</t>
         </is>
       </c>
     </row>
@@ -835,7 +915,12 @@
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>pago</t>
+          <t>Pago</t>
+        </is>
+      </c>
+      <c r="E17" t="inlineStr">
+        <is>
+          <t>-17%</t>
         </is>
       </c>
     </row>
@@ -859,7 +944,12 @@
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>pago</t>
+          <t>Pago</t>
+        </is>
+      </c>
+      <c r="E18" t="inlineStr">
+        <is>
+          <t>-4%</t>
         </is>
       </c>
     </row>
@@ -883,7 +973,12 @@
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>pago</t>
+          <t>Pago</t>
+        </is>
+      </c>
+      <c r="E19" t="inlineStr">
+        <is>
+          <t>-6%</t>
         </is>
       </c>
     </row>
@@ -907,7 +1002,12 @@
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>pago</t>
+          <t>Pago</t>
+        </is>
+      </c>
+      <c r="E20" t="inlineStr">
+        <is>
+          <t>-6%</t>
         </is>
       </c>
     </row>
@@ -919,19 +1019,24 @@
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>R$ 259,99</t>
+          <t>R$ 299,99</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
           <t>À vista no PIX
 ou até
-10x de R$ 30,58</t>
+10x de R$ 35,29</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>pago</t>
+          <t>Pago</t>
+        </is>
+      </c>
+      <c r="E21" t="inlineStr">
+        <is>
+          <t>0%</t>
         </is>
       </c>
     </row>
@@ -955,7 +1060,12 @@
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>pago</t>
+          <t>Pago</t>
+        </is>
+      </c>
+      <c r="E22" t="inlineStr">
+        <is>
+          <t>0%</t>
         </is>
       </c>
     </row>
@@ -979,950 +1089,1150 @@
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>pago</t>
+          <t>Pago</t>
+        </is>
+      </c>
+      <c r="E23" t="inlineStr">
+        <is>
+          <t>0%</t>
         </is>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>Gabinete Office Hayom GB1723, Micro-ATX, Mid Tower, Preto - GB.17.10.23</t>
+          <t>Mouse Lenovo USB, Essentials, 1600DPI, Preto</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>R$ 74,99</t>
+          <t>R$ 44,10</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
         <is>
           <t>À vista no PIX
 ou até
-3x de R$ 27,17</t>
+1x de R$ 44,10</t>
         </is>
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>pago</t>
+          <t>Grátis</t>
+        </is>
+      </c>
+      <c r="E24" t="inlineStr">
+        <is>
+          <t>0%</t>
         </is>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>Mouse Multi USB Emborrachado Preto - MO222</t>
+          <t>Gabinete Office Hayom GB1723, Micro-ATX, Mid Tower, Preto - GB.17.10.23</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>R$ 23,99</t>
+          <t>R$ 74,99</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
         <is>
           <t>À vista no PIX
 ou até
-1x de R$ 23,99</t>
+3x de R$ 27,17</t>
         </is>
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>pago</t>
+          <t>Pago</t>
+        </is>
+      </c>
+      <c r="E25" t="inlineStr">
+        <is>
+          <t>-11%</t>
         </is>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>Webcam Full HD Logitech C922 Pro Stream com Microfone Embutido, 1080p e Tripé Incluso, Compatível Logitech Capture - 960-001087</t>
+          <t>Mouse Multi USB Emborrachado Preto - MO222</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>R$ 599,90</t>
+          <t>R$ 23,99</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
         <is>
           <t>À vista no PIX
 ou até
-10x de R$ 63,14</t>
+1x de R$ 23,99</t>
         </is>
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>pago</t>
+          <t>Pago</t>
+        </is>
+      </c>
+      <c r="E26" t="inlineStr">
+        <is>
+          <t>0%</t>
         </is>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>Mouse sem fio Logitech MX Vertical Design Ergonômico para Redução de Tensão Muscular, USB Unifying ou Bluetooth, Recarregável - 910-005449</t>
+          <t>Webcam Full HD Logitech C922 Pro Stream com Microfone Embutido, 1080p e Tripé Incluso, Compatível Logitech Capture - 960-001087</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>R$ 479,99</t>
+          <t>R$ 599,90</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
         <is>
           <t>À vista no PIX
 ou até
-10x de R$ 52,17</t>
+10x de R$ 63,14</t>
         </is>
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t>pago</t>
+          <t>Grátis</t>
+        </is>
+      </c>
+      <c r="E27" t="inlineStr">
+        <is>
+          <t>-14%</t>
         </is>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>Headset Multi Pro, USB, Preto/Cinza - PH317</t>
+          <t>Mouse sem fio Logitech MX Vertical Design Ergonômico para Redução de Tensão Muscular, USB Unifying ou Bluetooth, Recarregável - 910-005449</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>R$ 119,90</t>
+          <t>R$ 479,99</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
         <is>
           <t>À vista no PIX
 ou até
-5x de R$ 28,21</t>
+10x de R$ 52,17</t>
         </is>
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>pago</t>
+          <t>Grátis</t>
+        </is>
+      </c>
+      <c r="E28" t="inlineStr">
+        <is>
+          <t>-7%</t>
         </is>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>Mouse sem fio Logitech M190 com Design Ambidestro de Tamanho Padrão, Conexão USB e Pilha Inclusa, Cinza - 910-005902</t>
+          <t>Headset Multi Pro, USB, Preto/Cinza - PH317</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>R$ 64,99</t>
+          <t>R$ 119,90</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
         <is>
           <t>À vista no PIX
 ou até
-2x de R$ 35,32</t>
+5x de R$ 28,21</t>
         </is>
       </c>
       <c r="D29" t="inlineStr">
         <is>
-          <t>pago</t>
+          <t>Pago</t>
+        </is>
+      </c>
+      <c r="E29" t="inlineStr">
+        <is>
+          <t>-14%</t>
         </is>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>Mouse Multi Classic Box Óptico Full Black - MO300</t>
+          <t>Mouse sem fio Logitech M190 com Design Ambidestro de Tamanho Padrão, Conexão USB e Pilha Inclusa, Cinza - 910-005902</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>R$ 8,00</t>
+          <t>R$ 64,99</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
         <is>
           <t>À vista no PIX
 ou até
-1x de R$ 8,00</t>
+2x de R$ 35,32</t>
         </is>
       </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t>pago</t>
+          <t>Pago</t>
+        </is>
+      </c>
+      <c r="E30" t="inlineStr">
+        <is>
+          <t>0%</t>
         </is>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>Mouse Sem Fio Logitech Signature M650, 2000 DPI, Compacto, 5 Botões, Silencioso, Bluetooth, USB, Grafite - 910-006250</t>
+          <t>Mouse Multi Classic Box Óptico Full Black - MO300</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>R$ 178,90</t>
+          <t>R$ 8,00</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
         <is>
           <t>À vista no PIX
 ou até
-7x de R$ 26,90</t>
+1x de R$ 8,00</t>
         </is>
       </c>
       <c r="D31" t="inlineStr">
         <is>
-          <t>pago</t>
+          <t>Pago</t>
+        </is>
+      </c>
+      <c r="E31" t="inlineStr">
+        <is>
+          <t>0%</t>
         </is>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>Mouse Sem Fio Logitech Signature M650 L 2000 DPI, Design Padrão, 5 Botões, Silencioso, Bluetooth, USB, Grafite - 910-006231</t>
+          <t>Mouse Sem Fio Logitech Signature M650, 2000 DPI, Compacto, 5 Botões, Silencioso, Bluetooth, USB, Grafite - 910-006250</t>
         </is>
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>R$ 188,99</t>
+          <t>R$ 175,99</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
         <is>
           <t>À vista no PIX
 ou até
-8x de R$ 26,84</t>
+7x de R$ 26,46</t>
         </is>
       </c>
       <c r="D32" t="inlineStr">
         <is>
-          <t>pago</t>
+          <t>Pago</t>
+        </is>
+      </c>
+      <c r="E32" t="inlineStr">
+        <is>
+          <t>0%</t>
         </is>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>Teclado Sem Fio Logitech Signature K650, Bluetooth, USB, Com Apoio para as Mãos, US, Grafite - 920-010911</t>
+          <t>Mouse Sem Fio Logitech Signature M650 L 2000 DPI, Design Padrão, 5 Botões, Silencioso, Bluetooth, USB, Grafite - 910-006231</t>
         </is>
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>R$ 259,99</t>
+          <t>R$ 188,99</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
         <is>
           <t>À vista no PIX
 ou até
-10x de R$ 30,58</t>
+8x de R$ 26,84</t>
         </is>
       </c>
       <c r="D33" t="inlineStr">
         <is>
-          <t>pago</t>
+          <t>Pago</t>
+        </is>
+      </c>
+      <c r="E33" t="inlineStr">
+        <is>
+          <t>0%</t>
         </is>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>Headset C3-Tech, USB, Preto - PH-340BK</t>
+          <t>Teclado Sem Fio Logitech Signature K650, Bluetooth, USB, Com Apoio para as Mãos, US, Grafite - 920-010911</t>
         </is>
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>R$ 97,90</t>
+          <t>R$ 259,99</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
         <is>
           <t>À vista no PIX
 ou até
-4x de R$ 28,79</t>
+10x de R$ 30,58</t>
         </is>
       </c>
       <c r="D34" t="inlineStr">
         <is>
-          <t>pago</t>
+          <t>Pago</t>
+        </is>
+      </c>
+      <c r="E34" t="inlineStr">
+        <is>
+          <t>0%</t>
         </is>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>Webcam Logitech C920e 1080p Vc 960-001401</t>
+          <t>Headset C3-Tech, USB, Preto - PH-340BK</t>
         </is>
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>R$ 443,70</t>
+          <t>R$ 97,90</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
         <is>
           <t>À vista no PIX
 ou até
-10x de R$ 52,20</t>
+4x de R$ 28,79</t>
         </is>
       </c>
       <c r="D35" t="inlineStr">
         <is>
-          <t>grátis</t>
+          <t>Pago</t>
+        </is>
+      </c>
+      <c r="E35" t="inlineStr">
+        <is>
+          <t>0%</t>
         </is>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>Headset Multi Pro, Driver 40mm, USB, Cabo 2M, Preto E Cinza - PH317</t>
+          <t>Webcam Logitech C920e 1080p Vc 960-001401</t>
         </is>
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>R$ 106,25</t>
+          <t>R$ 443,70</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
         <is>
           <t>À vista no PIX
 ou até
-5x de R$ 25,00</t>
+10x de R$ 52,20</t>
         </is>
       </c>
       <c r="D36" t="inlineStr">
         <is>
-          <t>grátis</t>
+          <t>Grátis</t>
+        </is>
+      </c>
+      <c r="E36" t="inlineStr">
+        <is>
+          <t>0%</t>
         </is>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>Teclado Multi Slim, USB, ABNT2, Teclas Silenciosas, Preto - TC213</t>
+          <t>Headset Multi Pro, Driver 40mm, USB, Cabo 2M, Preto E Cinza - PH317</t>
         </is>
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>R$ 26,90</t>
+          <t>R$ 106,25</t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
         <is>
           <t>À vista no PIX
 ou até
-1x de R$ 27,51</t>
+5x de R$ 25,00</t>
         </is>
       </c>
       <c r="D37" t="inlineStr">
         <is>
-          <t>pago</t>
+          <t>Grátis</t>
+        </is>
+      </c>
+      <c r="E37" t="inlineStr">
+        <is>
+          <t>0%</t>
         </is>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>Headset C3Tech Comfort com Microfone, Conexão P2, com Controle de Volume e Almofada de Espuma, Preto - PH-60BK</t>
+          <t>Teclado Multi Slim, USB, ABNT2, Teclas Silenciosas, Preto - TC213</t>
         </is>
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>R$ 41,99</t>
+          <t>R$ 26,90</t>
         </is>
       </c>
       <c r="C38" t="inlineStr">
         <is>
           <t>À vista no PIX
 ou até
-1x de R$ 44,46</t>
+1x de R$ 27,51</t>
         </is>
       </c>
       <c r="D38" t="inlineStr">
         <is>
-          <t>pago</t>
+          <t>Pago</t>
+        </is>
+      </c>
+      <c r="E38" t="inlineStr">
+        <is>
+          <t>0%</t>
         </is>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>Mouse Sem Fio Logitech Lift, 4000 DPI, 6 Botões, Bluetooth, Ergonômico, USB, Grafite - 910-006466</t>
+          <t>Headset C3Tech Comfort com Microfone, Conexão P2, com Controle de Volume e Almofada de Espuma, Preto - PH-60BK</t>
         </is>
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>R$ 319,99</t>
+          <t>R$ 41,99</t>
         </is>
       </c>
       <c r="C39" t="inlineStr">
         <is>
           <t>À vista no PIX
 ou até
-10x de R$ 34,78</t>
+1x de R$ 44,46</t>
         </is>
       </c>
       <c r="D39" t="inlineStr">
         <is>
-          <t>pago</t>
+          <t>Pago</t>
+        </is>
+      </c>
+      <c r="E39" t="inlineStr">
+        <is>
+          <t>-12%</t>
         </is>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>Headset Logitech H390, USB, com Almofadas, Controles de Áudio Integrado, Microfone com Redução de Ruído, Branco - 981-001285</t>
+          <t>Mouse Sem Fio Logitech Lift, 4000 DPI, 6 Botões, Bluetooth, Ergonômico, USB, Grafite - 910-006466</t>
         </is>
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>R$ 199,99</t>
+          <t>R$ 319,99</t>
         </is>
       </c>
       <c r="C40" t="inlineStr">
         <is>
           <t>À vista no PIX
 ou até
-8x de R$ 26,31</t>
+10x de R$ 34,78</t>
         </is>
       </c>
       <c r="D40" t="inlineStr">
         <is>
-          <t>pago</t>
+          <t>Grátis</t>
+        </is>
+      </c>
+      <c r="E40" t="inlineStr">
+        <is>
+          <t>-3%</t>
         </is>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>Headset Rise Mode Office 01, P3, Preto - RM-HS-OF-01-FB</t>
+          <t>Headset Sem Fio Logitech Zone Vibe 100, Drivers 40 mm, USB, Bluetooth, PC, Mobile, Grafite - 981-001214</t>
         </is>
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>R$ 42,99</t>
+          <t>R$ 589,99</t>
         </is>
       </c>
       <c r="C41" t="inlineStr">
         <is>
           <t>À vista no PIX
 ou até
-2x de R$ 25,29</t>
+10x de R$ 69,41</t>
         </is>
       </c>
       <c r="D41" t="inlineStr">
         <is>
-          <t>pago</t>
+          <t>Pago</t>
+        </is>
+      </c>
+      <c r="E41" t="inlineStr">
+        <is>
+          <t>0%</t>
         </is>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>Mouse Sem Fio Logitech M240, Bluetooth, Clique Silencioso, Design Ambidestro Compacto, Rosa - 910-007117</t>
+          <t>Headset Logitech H390, USB, com Almofadas, Controles de Áudio Integrado, Microfone com Redução de Ruído, Branco - 981-001285</t>
         </is>
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>R$ 74,90</t>
+          <t>R$ 199,99</t>
         </is>
       </c>
       <c r="C42" t="inlineStr">
         <is>
           <t>À vista no PIX
 ou até
-3x de R$ 26,28</t>
+8x de R$ 26,31</t>
         </is>
       </c>
       <c r="D42" t="inlineStr">
         <is>
-          <t>pago</t>
+          <t>Grátis</t>
+        </is>
+      </c>
+      <c r="E42" t="inlineStr">
+        <is>
+          <t>0%</t>
         </is>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>Teclado sem fio Logitech Signature Slim K950 Com Conexão Bluetooth ou Receptor USB Logi Bolt Incluso e Layout US INTL, Grafite - 920-012433</t>
+          <t>Headset Rise Mode Office 01, P3, Preto - RM-HS-OF-01-FB</t>
         </is>
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>R$ 435,99</t>
+          <t>R$ 42,99</t>
         </is>
       </c>
       <c r="C43" t="inlineStr">
         <is>
           <t>À vista no PIX
 ou até
-10x de R$ 51,29</t>
+2x de R$ 25,29</t>
         </is>
       </c>
       <c r="D43" t="inlineStr">
         <is>
-          <t>pago</t>
+          <t>Pago</t>
+        </is>
+      </c>
+      <c r="E43" t="inlineStr">
+        <is>
+          <t>-13%</t>
         </is>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>Teclado Slim Multi, USB, ABNT2, Resistente Água, Preto - TC065</t>
+          <t>Mouse Sem Fio Logitech M240, Bluetooth, Clique Silencioso, Design Ambidestro Compacto, Rosa - 910-007117</t>
         </is>
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>R$ 19,99</t>
+          <t>R$ 74,90</t>
         </is>
       </c>
       <c r="C44" t="inlineStr">
         <is>
           <t>À vista no PIX
 ou até
-1x de R$ 21,17</t>
+3x de R$ 26,28</t>
         </is>
       </c>
       <c r="D44" t="inlineStr">
         <is>
-          <t>pago</t>
+          <t>Pago</t>
+        </is>
+      </c>
+      <c r="E44" t="inlineStr">
+        <is>
+          <t>0%</t>
         </is>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>Mouse com fio USB Logitech M100 com Design Ambidestro e Facilidade Plug and Play, Cinza - 910-001601</t>
+          <t>Teclado sem fio Logitech Signature Slim K950 Com Conexão Bluetooth ou Receptor USB Logi Bolt Incluso e Layout US INTL, Grafite - 920-012433</t>
         </is>
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>R$ 41,90</t>
+          <t>R$ 435,99</t>
         </is>
       </c>
       <c r="C45" t="inlineStr">
         <is>
           <t>À vista no PIX
 ou até
-1x de R$ 44,36</t>
+10x de R$ 51,29</t>
         </is>
       </c>
       <c r="D45" t="inlineStr">
         <is>
-          <t>pago</t>
+          <t>Grátis</t>
+        </is>
+      </c>
+      <c r="E45" t="inlineStr">
+        <is>
+          <t>-12%</t>
         </is>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>Teclado sem fio Logitech K400 Plus TV com Touchpad Integrado, Conexão USB Unifying e Layout ABNT2 - 920-007125</t>
+          <t>Teclado Slim Multi, USB, ABNT2, Resistente Água, Preto - TC065</t>
         </is>
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>R$ 167,99</t>
+          <t>R$ 19,99</t>
         </is>
       </c>
       <c r="C46" t="inlineStr">
         <is>
           <t>À vista no PIX
 ou até
-7x de R$ 28,23</t>
+1x de R$ 21,17</t>
         </is>
       </c>
       <c r="D46" t="inlineStr">
         <is>
-          <t>pago</t>
+          <t>Pago</t>
+        </is>
+      </c>
+      <c r="E46" t="inlineStr">
+        <is>
+          <t>-39%</t>
         </is>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>Mouse Multi 1200DPI USB Preto - MO255</t>
+          <t>Mouse com fio USB Logitech M100 com Design Ambidestro e Facilidade Plug and Play, Cinza - 910-001601</t>
         </is>
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>R$ 15,90</t>
+          <t>R$ 41,90</t>
         </is>
       </c>
       <c r="C47" t="inlineStr">
         <is>
           <t>À vista no PIX
 ou até
-1x de R$ 16,84</t>
+1x de R$ 44,36</t>
         </is>
       </c>
       <c r="D47" t="inlineStr">
         <is>
-          <t>pago</t>
+          <t>Pago</t>
+        </is>
+      </c>
+      <c r="E47" t="inlineStr">
+        <is>
+          <t>0%</t>
         </is>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>Mouse Sem Fio Logitech Lift, 4000 DPI, 6 Botões, Bluetooth, Ergonômico, USB, Rose - 910-006472</t>
+          <t>Teclado sem fio Logitech K400 Plus TV com Touchpad Integrado, Conexão USB Unifying e Layout ABNT2 - 920-007125</t>
         </is>
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>R$ 319,99</t>
+          <t>R$ 167,99</t>
         </is>
       </c>
       <c r="C48" t="inlineStr">
         <is>
           <t>À vista no PIX
 ou até
-10x de R$ 37,64</t>
+7x de R$ 28,23</t>
         </is>
       </c>
       <c r="D48" t="inlineStr">
         <is>
-          <t>pago</t>
+          <t>Pago</t>
+        </is>
+      </c>
+      <c r="E48" t="inlineStr">
+        <is>
+          <t>0%</t>
         </is>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>Kit Teclado e Mouse Sem Fio Akko AKP104 WL, Bluetooth, ABNT2, Preto - 6975351383772</t>
+          <t>Mouse Multi 1200DPI USB Preto - MO255</t>
         </is>
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>R$ 99,99</t>
+          <t>R$ 15,90</t>
         </is>
       </c>
       <c r="C49" t="inlineStr">
         <is>
           <t>À vista no PIX
 ou até
-4x de R$ 29,41</t>
+1x de R$ 16,84</t>
         </is>
       </c>
       <c r="D49" t="inlineStr">
         <is>
-          <t>pago</t>
+          <t>Pago</t>
+        </is>
+      </c>
+      <c r="E49" t="inlineStr">
+        <is>
+          <t>0%</t>
         </is>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>Teclado e Mouse Sem Fio Multi Multimídia Slim 2.4Ghz ABNT2 Preto - TC183</t>
+          <t>Mouse Sem Fio Logitech Lift, 4000 DPI, 6 Botões, Bluetooth, Ergonômico, USB, Rose - 910-006472</t>
         </is>
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>R$ 69,99</t>
+          <t>R$ 319,99</t>
         </is>
       </c>
       <c r="C50" t="inlineStr">
         <is>
           <t>À vista no PIX
 ou até
-3x de R$ 27,44</t>
+10x de R$ 37,64</t>
         </is>
       </c>
       <c r="D50" t="inlineStr">
         <is>
-          <t>pago</t>
+          <t>Pago</t>
+        </is>
+      </c>
+      <c r="E50" t="inlineStr">
+        <is>
+          <t>0%</t>
         </is>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>Kit Multi Teclado e Mouse Sem Fio Slim, 1200 DPI, Conexão USB, ABNT2, Preto - TC212</t>
+          <t>Kit Teclado e Mouse Sem Fio Akko AKP104 WL, Bluetooth, ABNT2, Preto - 6975351383772</t>
         </is>
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>R$ 89,99</t>
+          <t>R$ 99,99</t>
         </is>
       </c>
       <c r="C51" t="inlineStr">
         <is>
           <t>À vista no PIX
 ou até
-4x de R$ 25,56</t>
+4x de R$ 29,41</t>
         </is>
       </c>
       <c r="D51" t="inlineStr">
         <is>
-          <t>pago</t>
+          <t>Pago</t>
+        </is>
+      </c>
+      <c r="E51" t="inlineStr">
+        <is>
+          <t>0%</t>
         </is>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
-          <t>Headset Fortrek Multimídia HBL-101 Preto/Prata - 62887</t>
+          <t>Teclado e Mouse Sem Fio Multi Multimídia Slim 2.4Ghz ABNT2 Preto - TC183</t>
         </is>
       </c>
       <c r="B52" t="inlineStr">
         <is>
-          <t>R$ 22,99</t>
+          <t>R$ 69,99</t>
         </is>
       </c>
       <c r="C52" t="inlineStr">
         <is>
           <t>À vista no PIX
 ou até
-1x de R$ 22,99</t>
+3x de R$ 27,44</t>
         </is>
       </c>
       <c r="D52" t="inlineStr">
         <is>
-          <t>pago</t>
+          <t>Pago</t>
+        </is>
+      </c>
+      <c r="E52" t="inlineStr">
+        <is>
+          <t>-18%</t>
         </is>
       </c>
     </row>
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
-          <t>Teclado Mecânico Sem Fio Logitech POP Keys, Switch Brown, Bluetooth, Teclas Emoji Personalizáveis, USB, Rosa Heartbreaker - 920-010712</t>
+          <t>Kit Multi Teclado e Mouse Sem Fio Slim, 1200 DPI, Conexão USB, ABNT2, Preto - TC212</t>
         </is>
       </c>
       <c r="B53" t="inlineStr">
         <is>
-          <t>R$ 569,90</t>
+          <t>R$ 89,99</t>
         </is>
       </c>
       <c r="C53" t="inlineStr">
         <is>
           <t>À vista no PIX
 ou até
-10x de R$ 59,98</t>
+4x de R$ 25,56</t>
         </is>
       </c>
       <c r="D53" t="inlineStr">
         <is>
-          <t>pago</t>
+          <t>Pago</t>
+        </is>
+      </c>
+      <c r="E53" t="inlineStr">
+        <is>
+          <t>-27%</t>
         </is>
       </c>
     </row>
     <row r="54">
       <c r="A54" t="inlineStr">
         <is>
-          <t>Teclado C3Tech Multimídia, com Fio, ABNT2, USB, Preto - KB-M40BK</t>
+          <t>Headset Fortrek Multimídia HBL-101 Preto/Prata - 62887</t>
         </is>
       </c>
       <c r="B54" t="inlineStr">
         <is>
-          <t>R$ 35,99</t>
+          <t>R$ 22,99</t>
         </is>
       </c>
       <c r="C54" t="inlineStr">
         <is>
           <t>À vista no PIX
 ou até
-1x de R$ 35,99</t>
+1x de R$ 22,99</t>
         </is>
       </c>
       <c r="D54" t="inlineStr">
         <is>
-          <t>pago</t>
+          <t>Pago</t>
+        </is>
+      </c>
+      <c r="E54" t="inlineStr">
+        <is>
+          <t>0%</t>
         </is>
       </c>
     </row>
     <row r="55">
       <c r="A55" t="inlineStr">
         <is>
-          <t>Headset Sem Fio Logitech Zone Vibe 100, Drivers 40 mm, USB, Bluetooth, PC, Mobile, Branco - 981-001218</t>
+          <t>Teclado Mecânico Sem Fio Logitech POP Keys, Switch Brown, Bluetooth, Teclas Emoji Personalizáveis, USB, Rosa Heartbreaker - 920-010712</t>
         </is>
       </c>
       <c r="B55" t="inlineStr">
         <is>
-          <t>R$ 499,90</t>
+          <t>R$ 569,90</t>
         </is>
       </c>
       <c r="C55" t="inlineStr">
         <is>
           <t>À vista no PIX
 ou até
-10x de R$ 58,81</t>
+10x de R$ 59,98</t>
         </is>
       </c>
       <c r="D55" t="inlineStr">
         <is>
-          <t>pago</t>
+          <t>Pago</t>
+        </is>
+      </c>
+      <c r="E55" t="inlineStr">
+        <is>
+          <t>-23%</t>
         </is>
       </c>
     </row>
     <row r="56">
       <c r="A56" t="inlineStr">
         <is>
-          <t>Teclado Sem Fio Logitech Wave Keys, Bluetooth, Layout US, Com Design Ondulado, Ergonômico, Grafite - 920-012281</t>
+          <t>Teclado C3Tech Multimídia, com Fio, ABNT2, USB, Preto - KB-M40BK</t>
         </is>
       </c>
       <c r="B56" t="inlineStr">
         <is>
-          <t>R$ 409,99</t>
+          <t>R$ 35,99</t>
         </is>
       </c>
       <c r="C56" t="inlineStr">
         <is>
           <t>À vista no PIX
 ou até
-10x de R$ 44,56</t>
+1x de R$ 35,99</t>
         </is>
       </c>
       <c r="D56" t="inlineStr">
         <is>
-          <t>pago</t>
+          <t>Pago</t>
+        </is>
+      </c>
+      <c r="E56" t="inlineStr">
+        <is>
+          <t>0%</t>
         </is>
       </c>
     </row>
     <row r="57">
       <c r="A57" t="inlineStr">
         <is>
-          <t>Teclado sem fio Logitech Signature Slim K950 Com Conexão Bluetooth ou Receptor USB Logi Bolt Incluso e Layout US INTL, Branco - 920-012601</t>
+          <t>Teclado Sem Fio Logitech Wave Keys, Bluetooth, Layout US, Com Design Ondulado, Ergonômico, Grafite - 920-012281</t>
         </is>
       </c>
       <c r="B57" t="inlineStr">
         <is>
-          <t>R$ 439,99</t>
+          <t>R$ 409,99</t>
         </is>
       </c>
       <c r="C57" t="inlineStr">
         <is>
           <t>À vista no PIX
 ou até
-10x de R$ 51,76</t>
+10x de R$ 44,56</t>
         </is>
       </c>
       <c r="D57" t="inlineStr">
         <is>
-          <t>pago</t>
+          <t>Pago</t>
+        </is>
+      </c>
+      <c r="E57" t="inlineStr">
+        <is>
+          <t>0%</t>
         </is>
       </c>
     </row>
     <row r="58">
       <c r="A58" t="inlineStr">
         <is>
-          <t>Headset Fortrek Multimídia HSL-102 Preto - 62889</t>
+          <t>Teclado sem fio Logitech Signature Slim K950 Com Conexão Bluetooth ou Receptor USB Logi Bolt Incluso e Layout US INTL, Branco - 920-012601</t>
         </is>
       </c>
       <c r="B58" t="inlineStr">
         <is>
-          <t>R$ 40,99</t>
+          <t>R$ 439,99</t>
         </is>
       </c>
       <c r="C58" t="inlineStr">
         <is>
           <t>À vista no PIX
 ou até
-1x de R$ 43,40</t>
+10x de R$ 51,76</t>
         </is>
       </c>
       <c r="D58" t="inlineStr">
         <is>
-          <t>pago</t>
+          <t>Grátis</t>
+        </is>
+      </c>
+      <c r="E58" t="inlineStr">
+        <is>
+          <t>0%</t>
         </is>
       </c>
     </row>
     <row r="59">
       <c r="A59" t="inlineStr">
         <is>
-          <t>Headset Bright Office, 2P2 - 0010</t>
+          <t>Headset Fortrek Multimídia HSL-102 Preto - 62889</t>
         </is>
       </c>
       <c r="B59" t="inlineStr">
         <is>
-          <t>R$ 19,99</t>
+          <t>R$ 40,99</t>
         </is>
       </c>
       <c r="C59" t="inlineStr">
         <is>
           <t>À vista no PIX
 ou até
-1x de R$ 21,17</t>
+1x de R$ 43,40</t>
         </is>
       </c>
       <c r="D59" t="inlineStr">
         <is>
-          <t>pago</t>
+          <t>Pago</t>
+        </is>
+      </c>
+      <c r="E59" t="inlineStr">
+        <is>
+          <t>0%</t>
         </is>
       </c>
     </row>
     <row r="60">
       <c r="A60" t="inlineStr">
         <is>
-          <t>Mesa Digitalizadora XP PEN Deco Mini 7, 5080LPI, 8 Teclas de Atalho, Caneta sem Bateria e 8192 Níveis de Sensibilidade - DECOMINI7</t>
+          <t>Headset Bright Office, 2P2 - 0010</t>
         </is>
       </c>
       <c r="B60" t="inlineStr">
         <is>
-          <t>R$ 279,99</t>
+          <t>R$ 19,99</t>
         </is>
       </c>
       <c r="C60" t="inlineStr">
         <is>
           <t>À vista no PIX
 ou até
-10x de R$ 32,94</t>
+1x de R$ 21,17</t>
         </is>
       </c>
       <c r="D60" t="inlineStr">
         <is>
-          <t>pago</t>
+          <t>Pago</t>
+        </is>
+      </c>
+      <c r="E60" t="inlineStr">
+        <is>
+          <t>0%</t>
         </is>
       </c>
     </row>
     <row r="61">
       <c r="A61" t="inlineStr">
         <is>
-          <t>Headset Maxprint Standard, com Microfone Ajustável, P2, Preto - 602314</t>
+          <t>Mesa Digitalizadora XP PEN Deco Mini 7, 5080LPI, 8 Teclas de Atalho, Caneta sem Bateria e 8192 Níveis de Sensibilidade - DECOMINI7</t>
         </is>
       </c>
       <c r="B61" t="inlineStr">
         <is>
-          <t>R$ 21,99</t>
+          <t>R$ 279,99</t>
         </is>
       </c>
       <c r="C61" t="inlineStr">
         <is>
           <t>À vista no PIX
 ou até
-1x de R$ 23,28</t>
+10x de R$ 32,94</t>
         </is>
       </c>
       <c r="D61" t="inlineStr">
         <is>
-          <t>pago</t>
+          <t>Pago</t>
+        </is>
+      </c>
+      <c r="E61" t="inlineStr">
+        <is>
+          <t>0%</t>
         </is>
       </c>
     </row>
     <row r="62">
       <c r="A62" t="inlineStr">
         <is>
-          <t>Mouse Sem Fio Logitech Signature M650, 2000 DPI, Compacto, 5 Botões, Silencioso, Bluetooth, USB, Rose - 910-006251</t>
+          <t>Headset Maxprint Standard, com Microfone Ajustável, P2, Preto - 602314</t>
         </is>
       </c>
       <c r="B62" t="inlineStr">
         <is>
-          <t>R$ 159,99</t>
+          <t>R$ 21,99</t>
         </is>
       </c>
       <c r="C62" t="inlineStr">
         <is>
           <t>À vista no PIX
 ou até
-6x de R$ 28,06</t>
+1x de R$ 23,28</t>
         </is>
       </c>
       <c r="D62" t="inlineStr">
         <is>
-          <t>pago</t>
+          <t>Pago</t>
+        </is>
+      </c>
+      <c r="E62" t="inlineStr">
+        <is>
+          <t>0%</t>
         </is>
       </c>
     </row>
     <row r="63">
       <c r="A63" t="inlineStr">
         <is>
-          <t>Mouse Sem Fio Logitech Signature M650, 2000 DPI, Compacto, 5 Botões, Silencioso, Bluetooth, USB, Branco - 910-006252</t>
+          <t>Mouse Sem Fio Logitech Signature M650, 2000 DPI, Compacto, 5 Botões, Silencioso, Bluetooth, USB, Rose - 910-006251</t>
         </is>
       </c>
       <c r="B63" t="inlineStr">
@@ -1934,1339 +2244,1619 @@
         <is>
           <t>À vista no PIX
 ou até
-7x de R$ 26,88</t>
+6x de R$ 28,06</t>
         </is>
       </c>
       <c r="D63" t="inlineStr">
         <is>
-          <t>pago</t>
+          <t>Pago</t>
+        </is>
+      </c>
+      <c r="E63" t="inlineStr">
+        <is>
+          <t>-10%</t>
         </is>
       </c>
     </row>
     <row r="64">
       <c r="A64" t="inlineStr">
         <is>
-          <t>Headset Sem Fio Logitech Zone Vibe 100, Drivers 40 mm, USB, Bluetooth, PC, Mobile, Rosa - 981-001223</t>
+          <t>Mouse Sem Fio Logitech Signature M650, 2000 DPI, Compacto, 5 Botões, Silencioso, Bluetooth, USB, Branco - 910-006252</t>
         </is>
       </c>
       <c r="B64" t="inlineStr">
         <is>
-          <t>R$ 649,99</t>
+          <t>R$ 159,99</t>
         </is>
       </c>
       <c r="C64" t="inlineStr">
         <is>
           <t>À vista no PIX
 ou até
-10x de R$ 76,46</t>
+7x de R$ 26,88</t>
         </is>
       </c>
       <c r="D64" t="inlineStr">
         <is>
-          <t>pago</t>
+          <t>Grátis</t>
+        </is>
+      </c>
+      <c r="E64" t="inlineStr">
+        <is>
+          <t>-20%</t>
         </is>
       </c>
     </row>
     <row r="65">
       <c r="A65" t="inlineStr">
         <is>
-          <t>Webcam Logitech Brio 300 Full HD, 1080p, 30 FPS, USB-C, Microfone Integrado, Grafite - 960-001413</t>
+          <t>Headset Sem Fio Logitech Zone Vibe 100, Drivers 40 mm, USB, Bluetooth, PC, Mobile, Rosa - 981-001223</t>
         </is>
       </c>
       <c r="B65" t="inlineStr">
         <is>
-          <t>R$ 419,99</t>
+          <t>R$ 649,99</t>
         </is>
       </c>
       <c r="C65" t="inlineStr">
         <is>
           <t>À vista no PIX
 ou até
-10x de R$ 49,41</t>
+10x de R$ 76,46</t>
         </is>
       </c>
       <c r="D65" t="inlineStr">
         <is>
-          <t>pago</t>
+          <t>Grátis</t>
+        </is>
+      </c>
+      <c r="E65" t="inlineStr">
+        <is>
+          <t>0%</t>
         </is>
       </c>
     </row>
     <row r="66">
       <c r="A66" t="inlineStr">
         <is>
-          <t>Teclado Sem Fio Multi TS400, Bluetooth, Preto - TC284</t>
+          <t>Webcam Logitech Brio 300 Full HD, 1080p, 30 FPS, USB-C, Microfone Integrado, Grafite - 960-001413</t>
         </is>
       </c>
       <c r="B66" t="inlineStr">
         <is>
-          <t>R$ 169,90</t>
+          <t>R$ 419,99</t>
         </is>
       </c>
       <c r="C66" t="inlineStr">
         <is>
           <t>À vista no PIX
 ou até
-7x de R$ 28,55</t>
+10x de R$ 49,41</t>
         </is>
       </c>
       <c r="D66" t="inlineStr">
         <is>
-          <t>pago</t>
+          <t>Grátis</t>
+        </is>
+      </c>
+      <c r="E66" t="inlineStr">
+        <is>
+          <t>0%</t>
         </is>
       </c>
     </row>
     <row r="67">
       <c r="A67" t="inlineStr">
         <is>
-          <t>Teclado e Mouse Sem Fio C3Tech, WiFi, Receptor USB, ABNT2, Preto - K-W60BK</t>
+          <t>Teclado Sem Fio Multi TS400, Bluetooth, Preto - TC284</t>
         </is>
       </c>
       <c r="B67" t="inlineStr">
         <is>
-          <t>R$ 93,99</t>
+          <t>R$ 169,90</t>
         </is>
       </c>
       <c r="C67" t="inlineStr">
         <is>
           <t>À vista no PIX
 ou até
-3x de R$ 32,97</t>
+7x de R$ 28,55</t>
         </is>
       </c>
       <c r="D67" t="inlineStr">
         <is>
-          <t>pago</t>
+          <t>Pago</t>
+        </is>
+      </c>
+      <c r="E67" t="inlineStr">
+        <is>
+          <t>0%</t>
         </is>
       </c>
     </row>
     <row r="68">
       <c r="A68" t="inlineStr">
         <is>
-          <t>Mouse Sem Fio Logitech Lift para Canhoto, 4000 DPI, 6 Botões, Bluetooth, Ergonômico, USB, Grafite - 910-006467</t>
+          <t>Teclado e Mouse Sem Fio C3Tech, WiFi, Receptor USB, ABNT2, Preto - K-W60BK</t>
         </is>
       </c>
       <c r="B68" t="inlineStr">
         <is>
-          <t>R$ 319,99</t>
+          <t>R$ 93,99</t>
         </is>
       </c>
       <c r="C68" t="inlineStr">
         <is>
           <t>À vista no PIX
 ou até
-10x de R$ 33,68</t>
+3x de R$ 32,97</t>
         </is>
       </c>
       <c r="D68" t="inlineStr">
         <is>
-          <t>pago</t>
+          <t>Pago</t>
+        </is>
+      </c>
+      <c r="E68" t="inlineStr">
+        <is>
+          <t>0%</t>
         </is>
       </c>
     </row>
     <row r="69">
       <c r="A69" t="inlineStr">
         <is>
-          <t>Headset Sem Fio Logitech Zone 300 Com Microfone com Cancelamento de Ruído, Conexão Bluetooth, Bateria Recarregável via USB-C, Rosa - 981-001411</t>
+          <t>Mouse Sem Fio Logitech Lift para Canhoto, 4000 DPI, 6 Botões, Bluetooth, Ergonômico, USB, Grafite - 910-006467</t>
         </is>
       </c>
       <c r="B69" t="inlineStr">
         <is>
-          <t>R$ 349,99</t>
+          <t>R$ 319,99</t>
         </is>
       </c>
       <c r="C69" t="inlineStr">
         <is>
           <t>À vista no PIX
 ou até
-10x de R$ 41,17</t>
+10x de R$ 33,68</t>
         </is>
       </c>
       <c r="D69" t="inlineStr">
         <is>
-          <t>grátis</t>
+          <t>Grátis</t>
+        </is>
+      </c>
+      <c r="E69" t="inlineStr">
+        <is>
+          <t>0%</t>
         </is>
       </c>
     </row>
     <row r="70">
       <c r="A70" t="inlineStr">
         <is>
-          <t>Mouse Sem Fio Intelbras MSI 200, 2.4Hz, 6 Botões, Preto - 4290024</t>
+          <t>Headset Sem Fio Logitech Zone 300 Com Microfone com Cancelamento de Ruído, Conexão Bluetooth, Bateria Recarregável via USB-C, Rosa - 981-001411</t>
         </is>
       </c>
       <c r="B70" t="inlineStr">
         <is>
-          <t>R$ 68,99</t>
+          <t>R$ 349,99</t>
         </is>
       </c>
       <c r="C70" t="inlineStr">
         <is>
           <t>À vista no PIX
 ou até
-2x de R$ 37,49</t>
+10x de R$ 41,17</t>
         </is>
       </c>
       <c r="D70" t="inlineStr">
         <is>
-          <t>pago</t>
+          <t>Grátis</t>
+        </is>
+      </c>
+      <c r="E70" t="inlineStr">
+        <is>
+          <t>-18%</t>
         </is>
       </c>
     </row>
     <row r="71">
       <c r="A71" t="inlineStr">
         <is>
-          <t>Mesa Digitalizadora Com Tela Wacom Movink, Caneta Pro Pen 3, 5080 LPI, 13", Full HD, Preto - DTH135K0A</t>
+          <t>Mouse Sem Fio Intelbras MSI 200, 2.4Hz, 6 Botões, Preto - 4290024</t>
         </is>
       </c>
       <c r="B71" t="inlineStr">
         <is>
-          <t>R$ 5.699,99</t>
+          <t>R$ 68,99</t>
         </is>
       </c>
       <c r="C71" t="inlineStr">
         <is>
           <t>À vista no PIX
 ou até
-10x de R$ 670,58</t>
+2x de R$ 37,49</t>
         </is>
       </c>
       <c r="D71" t="inlineStr">
         <is>
-          <t>pago</t>
+          <t>Pago</t>
+        </is>
+      </c>
+      <c r="E71" t="inlineStr">
+        <is>
+          <t>0%</t>
         </is>
       </c>
     </row>
     <row r="72">
       <c r="A72" t="inlineStr">
         <is>
-          <t>Webcam Razer Kiyo X, Full HD, 30FPS, Preto - RZ1904170100R3U</t>
+          <t>Mesa Digitalizadora Com Tela Wacom Movink, Caneta Pro Pen 3, 5080 LPI, 13", Full HD, Preto - DTH135K0A</t>
         </is>
       </c>
       <c r="B72" t="inlineStr">
         <is>
-          <t>R$ 679,99</t>
+          <t>R$ 5.699,99</t>
         </is>
       </c>
       <c r="C72" t="inlineStr">
         <is>
           <t>À vista no PIX
 ou até
-10x de R$ 79,99</t>
+10x de R$ 670,58</t>
         </is>
       </c>
       <c r="D72" t="inlineStr">
         <is>
-          <t>pago</t>
+          <t>Pago</t>
+        </is>
+      </c>
+      <c r="E72" t="inlineStr">
+        <is>
+          <t>0%</t>
         </is>
       </c>
     </row>
     <row r="73">
       <c r="A73" t="inlineStr">
         <is>
-          <t>Headset Poly Blackwire 3325 Stereo, USB-C/A, Preto - 8X222AA</t>
+          <t>Webcam Razer Kiyo X, Full HD, 30FPS, Preto - RZ1904170100R3U</t>
         </is>
       </c>
       <c r="B73" t="inlineStr">
         <is>
-          <t>R$ 499,99</t>
+          <t>R$ 679,99</t>
         </is>
       </c>
       <c r="C73" t="inlineStr">
         <is>
           <t>À vista no PIX
 ou até
-10x de R$ 55,55</t>
+10x de R$ 79,99</t>
         </is>
       </c>
       <c r="D73" t="inlineStr">
         <is>
-          <t>pago</t>
+          <t>Pago</t>
+        </is>
+      </c>
+      <c r="E73" t="inlineStr">
+        <is>
+          <t>0%</t>
         </is>
       </c>
     </row>
     <row r="74">
       <c r="A74" t="inlineStr">
         <is>
-          <t>Teclado Sem Fio Logitech Keys-To-Go 2, Bluetooth, para Tablets, iPad, macOs, Windows, Capa Integrada, Grafite - 920-012867</t>
+          <t>Headset Poly Blackwire 3325 Stereo, USB-C/A, Preto - 8X222AA</t>
         </is>
       </c>
       <c r="B74" t="inlineStr">
         <is>
-          <t>R$ 509,90</t>
+          <t>R$ 499,99</t>
         </is>
       </c>
       <c r="C74" t="inlineStr">
         <is>
           <t>À vista no PIX
 ou até
-10x de R$ 59,98</t>
+10x de R$ 55,55</t>
         </is>
       </c>
       <c r="D74" t="inlineStr">
         <is>
-          <t>pago</t>
+          <t>Pago</t>
+        </is>
+      </c>
+      <c r="E74" t="inlineStr">
+        <is>
+          <t>0%</t>
         </is>
       </c>
     </row>
     <row r="75">
       <c r="A75" t="inlineStr">
         <is>
-          <t>Mouse Multi Com Fio 1600Dpi USB 6 Botões Preto MO241</t>
+          <t>Teclado Sem Fio Logitech Keys-To-Go 2, Bluetooth, para Tablets, iPad, macOs, Windows, Capa Integrada, Grafite - 920-012867</t>
         </is>
       </c>
       <c r="B75" t="inlineStr">
         <is>
-          <t>R$ 25,99</t>
+          <t>R$ 509,90</t>
         </is>
       </c>
       <c r="C75" t="inlineStr">
         <is>
           <t>À vista no PIX
 ou até
-1x de R$ 26,58</t>
+10x de R$ 59,98</t>
         </is>
       </c>
       <c r="D75" t="inlineStr">
         <is>
-          <t>pago</t>
+          <t>Grátis</t>
+        </is>
+      </c>
+      <c r="E75" t="inlineStr">
+        <is>
+          <t>0%</t>
         </is>
       </c>
     </row>
     <row r="76">
       <c r="A76" t="inlineStr">
         <is>
-          <t>Headset Logitech H390, USB, com Almofadas, Controles de Áudio Integrado, Microfone com Redução de Ruído, Rosa - 981-001280</t>
+          <t>Mouse Multi Com Fio 1600Dpi USB 6 Botões Preto MO241</t>
         </is>
       </c>
       <c r="B76" t="inlineStr">
         <is>
-          <t>R$ 179,90</t>
+          <t>R$ 25,99</t>
         </is>
       </c>
       <c r="C76" t="inlineStr">
         <is>
           <t>À vista no PIX
 ou até
-8x de R$ 26,45</t>
+1x de R$ 26,58</t>
         </is>
       </c>
       <c r="D76" t="inlineStr">
         <is>
-          <t>pago</t>
+          <t>Pago</t>
+        </is>
+      </c>
+      <c r="E76" t="inlineStr">
+        <is>
+          <t>-21%</t>
         </is>
       </c>
     </row>
     <row r="77">
       <c r="A77" t="inlineStr">
         <is>
-          <t>Webcam Logitech Brio 300 Full HD, 1080p, 30 FPS, USB-C, Microfone Integrado, Branco - 960-001440</t>
+          <t>Mouse com fio USB Logitech M110 com Clique Silencioso, Design Ambidestro e Facilidade Plug and Play, Vermelho - 910-006755</t>
         </is>
       </c>
       <c r="B77" t="inlineStr">
         <is>
-          <t>R$ 399,99</t>
+          <t>R$ 48,99</t>
         </is>
       </c>
       <c r="C77" t="inlineStr">
         <is>
           <t>À vista no PIX
 ou até
-10x de R$ 47,05</t>
+2x de R$ 28,82</t>
         </is>
       </c>
       <c r="D77" t="inlineStr">
         <is>
-          <t>pago</t>
+          <t>Pago</t>
+        </is>
+      </c>
+      <c r="E77" t="inlineStr">
+        <is>
+          <t>0%</t>
         </is>
       </c>
     </row>
     <row r="78">
       <c r="A78" t="inlineStr">
         <is>
-          <t>Mouse Sem Fio Multi MS300, 1200DPI, USB, 3 Botões, Preto - MO380</t>
+          <t>Headset Logitech H390, USB, com Almofadas, Controles de Áudio Integrado, Microfone com Redução de Ruído, Rosa - 981-001280</t>
         </is>
       </c>
       <c r="B78" t="inlineStr">
         <is>
-          <t>R$ 38,99</t>
+          <t>R$ 179,90</t>
         </is>
       </c>
       <c r="C78" t="inlineStr">
         <is>
           <t>À vista no PIX
 ou até
-1x de R$ 38,99</t>
+8x de R$ 26,45</t>
         </is>
       </c>
       <c r="D78" t="inlineStr">
         <is>
-          <t>pago</t>
+          <t>Grátis</t>
+        </is>
+      </c>
+      <c r="E78" t="inlineStr">
+        <is>
+          <t>-18%</t>
         </is>
       </c>
     </row>
     <row r="79">
       <c r="A79" t="inlineStr">
         <is>
-          <t>Mouse Multi MF400, 1200DPI, USB, 3 Botões, Cinza - MO387</t>
+          <t>Webcam Logitech Brio 300 Full HD, 1080p, 30 FPS, USB-C, Microfone Integrado, Branco - 960-001440</t>
         </is>
       </c>
       <c r="B79" t="inlineStr">
         <is>
-          <t>R$ 25,90</t>
+          <t>R$ 399,99</t>
         </is>
       </c>
       <c r="C79" t="inlineStr">
         <is>
           <t>À vista no PIX
 ou até
-1x de R$ 26,49</t>
+10x de R$ 47,05</t>
         </is>
       </c>
       <c r="D79" t="inlineStr">
         <is>
-          <t>pago</t>
+          <t>Pago</t>
+        </is>
+      </c>
+      <c r="E79" t="inlineStr">
+        <is>
+          <t>0%</t>
         </is>
       </c>
     </row>
     <row r="80">
       <c r="A80" t="inlineStr">
         <is>
-          <t>Mesa Digitalizadora Com Tela XP-Pen, Magic Drawing PAD, Com Caneta, 2540 LPI, QHD, USB-C</t>
+          <t>Mouse Sem Fio Multi MS300, 1200DPI, USB, 3 Botões, Preto - MO380</t>
         </is>
       </c>
       <c r="B80" t="inlineStr">
         <is>
-          <t>R$ 4.459,99</t>
+          <t>R$ 38,99</t>
         </is>
       </c>
       <c r="C80" t="inlineStr">
         <is>
           <t>À vista no PIX
 ou até
-10x de R$ 524,70</t>
+1x de R$ 38,99</t>
         </is>
       </c>
       <c r="D80" t="inlineStr">
         <is>
-          <t>pago</t>
+          <t>Pago</t>
+        </is>
+      </c>
+      <c r="E80" t="inlineStr">
+        <is>
+          <t>0%</t>
         </is>
       </c>
     </row>
     <row r="81">
       <c r="A81" t="inlineStr">
         <is>
-          <t>Headset Poly Blackwire 3320, USB-C, Preto - 8X220AA</t>
+          <t>Mouse Multi MF400, 1200DPI, USB, 3 Botões, Cinza - MO387</t>
         </is>
       </c>
       <c r="B81" t="inlineStr">
         <is>
-          <t>R$ 402,86</t>
+          <t>R$ 25,90</t>
         </is>
       </c>
       <c r="C81" t="inlineStr">
         <is>
           <t>À vista no PIX
 ou até
-10x de R$ 44,76</t>
+1x de R$ 26,49</t>
         </is>
       </c>
       <c r="D81" t="inlineStr">
         <is>
-          <t>pago</t>
+          <t>Pago</t>
+        </is>
+      </c>
+      <c r="E81" t="inlineStr">
+        <is>
+          <t>0%</t>
         </is>
       </c>
     </row>
     <row r="82">
       <c r="A82" t="inlineStr">
         <is>
-          <t>Headset Sem Fio Poly Voyager Focus 2, USB, Bluetooth, Preto - 77Y88AA</t>
+          <t>Mesa Digitalizadora Com Tela XP-Pen, Magic Drawing PAD, Com Caneta, 2540 LPI, QHD, USB-C</t>
         </is>
       </c>
       <c r="B82" t="inlineStr">
         <is>
-          <t>R$ 1.699,99</t>
+          <t>R$ 4.459,99</t>
         </is>
       </c>
       <c r="C82" t="inlineStr">
         <is>
           <t>À vista no PIX
 ou até
-10x de R$ 188,88</t>
+10x de R$ 524,70</t>
         </is>
       </c>
       <c r="D82" t="inlineStr">
         <is>
-          <t>pago</t>
+          <t>Pago</t>
+        </is>
+      </c>
+      <c r="E82" t="inlineStr">
+        <is>
+          <t>-5%</t>
         </is>
       </c>
     </row>
     <row r="83">
       <c r="A83" t="inlineStr">
         <is>
-          <t>Mochila Acer para Notebook até 15,6´ - NP.BAG1A.269</t>
+          <t>Headset Poly Blackwire 3320, USB-C, Preto - 8X220AA</t>
         </is>
       </c>
       <c r="B83" t="inlineStr">
         <is>
-          <t>R$ 199,99</t>
+          <t>R$ 402,86</t>
         </is>
       </c>
       <c r="C83" t="inlineStr">
         <is>
           <t>À vista no PIX
 ou até
-9x de R$ 26,14</t>
+10x de R$ 44,76</t>
         </is>
       </c>
       <c r="D83" t="inlineStr">
         <is>
-          <t>pago</t>
+          <t>Pago</t>
+        </is>
+      </c>
+      <c r="E83" t="inlineStr">
+        <is>
+          <t>0%</t>
         </is>
       </c>
     </row>
     <row r="84">
       <c r="A84" t="inlineStr">
         <is>
-          <t>Headset Jabra Evolve 40 Duo, Microfone, USB, Preto - 6399-823-109</t>
+          <t>Headset Sem Fio Poly Voyager Focus 2, USB, Bluetooth, Preto - 77Y88AA</t>
         </is>
       </c>
       <c r="B84" t="inlineStr">
         <is>
-          <t>R$ 899,99</t>
+          <t>R$ 1.699,99</t>
         </is>
       </c>
       <c r="C84" t="inlineStr">
         <is>
           <t>À vista no PIX
 ou até
-10x de R$ 99,99</t>
+10x de R$ 188,88</t>
         </is>
       </c>
       <c r="D84" t="inlineStr">
         <is>
-          <t>pago</t>
+          <t>Pago</t>
+        </is>
+      </c>
+      <c r="E84" t="inlineStr">
+        <is>
+          <t>0%</t>
         </is>
       </c>
     </row>
     <row r="85">
       <c r="A85" t="inlineStr">
         <is>
-          <t>Headset PH-G12 C3Tech, P2, PS4, Drivers 40mm, Preto - PH-G12BK</t>
+          <t>Mochila Acer para Notebook até 15,6´ - NP.BAG1A.269</t>
         </is>
       </c>
       <c r="B85" t="inlineStr">
         <is>
-          <t>R$ 78,90</t>
+          <t>R$ 199,99</t>
         </is>
       </c>
       <c r="C85" t="inlineStr">
         <is>
           <t>À vista no PIX
 ou até
-3x de R$ 28,58</t>
+9x de R$ 26,14</t>
         </is>
       </c>
       <c r="D85" t="inlineStr">
         <is>
-          <t>pago</t>
+          <t>Pago</t>
+        </is>
+      </c>
+      <c r="E85" t="inlineStr">
+        <is>
+          <t>0%</t>
         </is>
       </c>
     </row>
     <row r="86">
       <c r="A86" t="inlineStr">
         <is>
-          <t>Headset Felitron Bravo, USB Stereo, Driver 60mm, Preto - 01183-2</t>
+          <t>Headset Jabra Evolve 40 Duo, Microfone, USB, Preto - 6399-823-109</t>
         </is>
       </c>
       <c r="B86" t="inlineStr">
         <is>
-          <t>R$ 234,99</t>
+          <t>R$ 899,99</t>
         </is>
       </c>
       <c r="C86" t="inlineStr">
         <is>
           <t>À vista no PIX
 ou até
-10x de R$ 27,64</t>
+10x de R$ 99,99</t>
         </is>
       </c>
       <c r="D86" t="inlineStr">
         <is>
-          <t>pago</t>
+          <t>Pago</t>
+        </is>
+      </c>
+      <c r="E86" t="inlineStr">
+        <is>
+          <t>0%</t>
         </is>
       </c>
     </row>
     <row r="87">
       <c r="A87" t="inlineStr">
         <is>
-          <t>Headset Dahua, Controles de Áudio Integrado e Microfone, USB, Preto - VCS-ER200</t>
+          <t>Headset PH-G12 C3Tech, P2, PS4, Drivers 40mm, Preto - PH-G12BK</t>
         </is>
       </c>
       <c r="B87" t="inlineStr">
         <is>
-          <t>R$ 539,99</t>
+          <t>R$ 78,90</t>
         </is>
       </c>
       <c r="C87" t="inlineStr">
         <is>
           <t>À vista no PIX
 ou até
-10x de R$ 63,52</t>
+3x de R$ 28,58</t>
         </is>
       </c>
       <c r="D87" t="inlineStr">
         <is>
-          <t>pago</t>
+          <t>Pago</t>
+        </is>
+      </c>
+      <c r="E87" t="inlineStr">
+        <is>
+          <t>0%</t>
         </is>
       </c>
     </row>
     <row r="88">
       <c r="A88" t="inlineStr">
         <is>
-          <t>Fone de Ouvido Sem Fio Poly VFocus2-M, Bluetooth, Preto - 77Y90AA</t>
+          <t>Headset Felitron Bravo, USB Stereo, Driver 60mm, Preto - 01183-2</t>
         </is>
       </c>
       <c r="B88" t="inlineStr">
         <is>
-          <t>R$ 1.899,99</t>
+          <t>R$ 234,99</t>
         </is>
       </c>
       <c r="C88" t="inlineStr">
         <is>
           <t>À vista no PIX
 ou até
-10x de R$ 206,52</t>
+10x de R$ 27,64</t>
         </is>
       </c>
       <c r="D88" t="inlineStr">
         <is>
-          <t>pago</t>
+          <t>Pago</t>
+        </is>
+      </c>
+      <c r="E88" t="inlineStr">
+        <is>
+          <t>0%</t>
         </is>
       </c>
     </row>
     <row r="89">
       <c r="A89" t="inlineStr">
         <is>
-          <t>Headset Poly Blackwire 3225, USB, USB-C, Preto - 8X229A6</t>
+          <t>Headset Dahua, Controles de Áudio Integrado e Microfone, USB, Preto - VCS-ER200</t>
         </is>
       </c>
       <c r="B89" t="inlineStr">
         <is>
-          <t>R$ 449,90</t>
+          <t>R$ 539,99</t>
         </is>
       </c>
       <c r="C89" t="inlineStr">
         <is>
           <t>À vista no PIX
 ou até
-10x de R$ 49,98</t>
+10x de R$ 63,52</t>
         </is>
       </c>
       <c r="D89" t="inlineStr">
         <is>
-          <t>pago</t>
+          <t>Pago</t>
+        </is>
+      </c>
+      <c r="E89" t="inlineStr">
+        <is>
+          <t>0%</t>
         </is>
       </c>
     </row>
     <row r="90">
       <c r="A90" t="inlineStr">
         <is>
-          <t>Headset Sem Fio HP Poly Voyager Focus 2, USB-A, Adaptador USB BT700 Bluetooth + Base de Carregamento, Preto - 77Y86AA</t>
+          <t>Fone de Ouvido Sem Fio Poly VFocus2-M, Bluetooth, Preto - 77Y90AA</t>
         </is>
       </c>
       <c r="B90" t="inlineStr">
         <is>
-          <t>R$ 1.562,99</t>
+          <t>R$ 1.899,99</t>
         </is>
       </c>
       <c r="C90" t="inlineStr">
         <is>
           <t>À vista no PIX
 ou até
-10x de R$ 173,66</t>
+10x de R$ 206,52</t>
         </is>
       </c>
       <c r="D90" t="inlineStr">
         <is>
-          <t>pago</t>
+          <t>Pago</t>
+        </is>
+      </c>
+      <c r="E90" t="inlineStr">
+        <is>
+          <t>0%</t>
         </is>
       </c>
     </row>
     <row r="91">
       <c r="A91" t="inlineStr">
         <is>
-          <t>Headset Sem Fio Dell WL3024, Cancelamento de Ruído, Recarregável, Preto - 520-BBCH</t>
+          <t>Headset Poly Blackwire 3225, USB, USB-C, Preto - 8X229A6</t>
         </is>
       </c>
       <c r="B91" t="inlineStr">
         <is>
-          <t>R$ 1.059,00</t>
+          <t>R$ 449,90</t>
         </is>
       </c>
       <c r="C91" t="inlineStr">
         <is>
           <t>À vista no PIX
 ou até
-10x de R$ 117,66</t>
+10x de R$ 49,98</t>
         </is>
       </c>
       <c r="D91" t="inlineStr">
         <is>
-          <t>pago</t>
+          <t>Pago</t>
+        </is>
+      </c>
+      <c r="E91" t="inlineStr">
+        <is>
+          <t>-4%</t>
         </is>
       </c>
     </row>
     <row r="92">
       <c r="A92" t="inlineStr">
         <is>
-          <t>Cabo Fonte Sleeved Rise Mode Preto e Branco - RM-SL-BW</t>
+          <t>Headset Sem Fio HP Poly Voyager Focus 2, USB-A, Adaptador USB BT700 Bluetooth + Base de Carregamento, Preto - 77Y86AA</t>
         </is>
       </c>
       <c r="B92" t="inlineStr">
         <is>
-          <t>R$ 94,99</t>
+          <t>R$ 1.562,99</t>
         </is>
       </c>
       <c r="C92" t="inlineStr">
         <is>
           <t>À vista no PIX
 ou até
-4x de R$ 27,93</t>
+10x de R$ 173,66</t>
         </is>
       </c>
       <c r="D92" t="inlineStr">
         <is>
-          <t>pago</t>
+          <t>Pago</t>
+        </is>
+      </c>
+      <c r="E92" t="inlineStr">
+        <is>
+          <t>-2%</t>
         </is>
       </c>
     </row>
     <row r="93">
       <c r="A93" t="inlineStr">
         <is>
-          <t>Cabo Fonte Sleeved Rise Mode Full Red Vermelho - RM-SL-FR</t>
+          <t>Headset Sem Fio Dell WL3024, Cancelamento de Ruído, Recarregável, Preto - 520-BBCH</t>
         </is>
       </c>
       <c r="B93" t="inlineStr">
         <is>
-          <t>R$ 79,99</t>
+          <t>R$ 1.059,00</t>
         </is>
       </c>
       <c r="C93" t="inlineStr">
         <is>
           <t>À vista no PIX
 ou até
-3x de R$ 31,37</t>
+10x de R$ 117,66</t>
         </is>
       </c>
       <c r="D93" t="inlineStr">
         <is>
-          <t>pago</t>
+          <t>Pago</t>
+        </is>
+      </c>
+      <c r="E93" t="inlineStr">
+        <is>
+          <t>0%</t>
         </is>
       </c>
     </row>
     <row r="94">
       <c r="A94" t="inlineStr">
         <is>
-          <t>Pen Drive 128GB Kingston DataTraveler Exodia, USB 3.2, Preto e Amarelo - DTX/128GB</t>
+          <t>Cabo Fonte Sleeved Rise Mode Preto e Branco - RM-SL-BW</t>
         </is>
       </c>
       <c r="B94" t="inlineStr">
         <is>
-          <t>R$ 52,99</t>
+          <t>R$ 94,99</t>
         </is>
       </c>
       <c r="C94" t="inlineStr">
         <is>
           <t>À vista no PIX
 ou até
-2x de R$ 31,17</t>
+4x de R$ 27,93</t>
         </is>
       </c>
       <c r="D94" t="inlineStr">
         <is>
-          <t>pago</t>
+          <t>Pago</t>
+        </is>
+      </c>
+      <c r="E94" t="inlineStr">
+        <is>
+          <t>-20%</t>
         </is>
       </c>
     </row>
     <row r="95">
       <c r="A95" t="inlineStr">
         <is>
-          <t>Teclado Sem Fio Logitech MX Keys Mini, Iluminação Smart, Bluetooth, USB, Easy-Switch, Recarregável, Cinza Claro - 920-010506</t>
+          <t>Cabo Fonte Sleeved Rise Mode Full Red Vermelho - RM-SL-FR</t>
         </is>
       </c>
       <c r="B95" t="inlineStr">
         <is>
-          <t>R$ 649,99</t>
+          <t>R$ 79,99</t>
         </is>
       </c>
       <c r="C95" t="inlineStr">
         <is>
           <t>À vista no PIX
 ou até
-10x de R$ 76,46</t>
+3x de R$ 31,37</t>
         </is>
       </c>
       <c r="D95" t="inlineStr">
         <is>
-          <t>pago</t>
+          <t>Pago</t>
+        </is>
+      </c>
+      <c r="E95" t="inlineStr">
+        <is>
+          <t>-20%</t>
         </is>
       </c>
     </row>
     <row r="96">
       <c r="A96" t="inlineStr">
         <is>
-          <t>Mesa Digitalizadora Huion Kamvas Plus 24", Tela QHD 2.5K IPS, 5080 LPI, USB-C, USB, Preto - GS2402</t>
+          <t>Pen Drive 128GB Kingston DataTraveler Exodia, USB 3.2, Preto e Amarelo - DTX/128GB</t>
         </is>
       </c>
       <c r="B96" t="inlineStr">
         <is>
-          <t>R$ 5.399,99</t>
+          <t>R$ 52,99</t>
         </is>
       </c>
       <c r="C96" t="inlineStr">
         <is>
           <t>À vista no PIX
 ou até
-10x de R$ 635,29</t>
+2x de R$ 31,17</t>
         </is>
       </c>
       <c r="D96" t="inlineStr">
         <is>
-          <t>pago</t>
+          <t>Pago</t>
+        </is>
+      </c>
+      <c r="E96" t="inlineStr">
+        <is>
+          <t>-33%</t>
         </is>
       </c>
     </row>
     <row r="97">
       <c r="A97" t="inlineStr">
         <is>
-          <t>Base com Cooler para Notebook Rise Mode, Galaxy Black X4, LED - RM-CN-04-BB</t>
+          <t>Teclado Sem Fio Logitech MX Keys Mini, Iluminação Smart, Bluetooth, USB, Easy-Switch, Recarregável, Cinza Claro - 920-010506</t>
         </is>
       </c>
       <c r="B97" t="inlineStr">
         <is>
-          <t>R$ 39,99</t>
+          <t>R$ 649,99</t>
         </is>
       </c>
       <c r="C97" t="inlineStr">
         <is>
           <t>À vista no PIX
 ou até
-1x de R$ 42,34</t>
+10x de R$ 76,46</t>
         </is>
       </c>
       <c r="D97" t="inlineStr">
         <is>
-          <t>pago</t>
+          <t>Grátis</t>
+        </is>
+      </c>
+      <c r="E97" t="inlineStr">
+        <is>
+          <t>0%</t>
         </is>
       </c>
     </row>
     <row r="98">
       <c r="A98" t="inlineStr">
         <is>
-          <t>Base com Cooler para Notebook Rise Mode, Galaxy Black X6, LED - RM-CN-06-BB</t>
+          <t>Mesa Digitalizadora Huion Kamvas Plus 24", Tela QHD 2.5K IPS, 5080 LPI, USB-C, USB, Preto - GS2402</t>
         </is>
       </c>
       <c r="B98" t="inlineStr">
         <is>
-          <t>R$ 36,99</t>
+          <t>R$ 5.399,99</t>
         </is>
       </c>
       <c r="C98" t="inlineStr">
         <is>
           <t>À vista no PIX
 ou até
-1x de R$ 39,17</t>
+10x de R$ 635,29</t>
         </is>
       </c>
       <c r="D98" t="inlineStr">
         <is>
-          <t>pago</t>
+          <t>Pago</t>
+        </is>
+      </c>
+      <c r="E98" t="inlineStr">
+        <is>
+          <t>-7%</t>
         </is>
       </c>
     </row>
     <row r="99">
       <c r="A99" t="inlineStr">
         <is>
-          <t>Pen Drive 64GB Kingston DataTraveler Exodia Onyx, USB 3.2, Preto - DTXON/64GB</t>
+          <t>Base com Cooler para Notebook Rise Mode, Galaxy Black X4, LED - RM-CN-04-BB</t>
         </is>
       </c>
       <c r="B99" t="inlineStr">
         <is>
-          <t>R$ 38,99</t>
+          <t>R$ 39,99</t>
         </is>
       </c>
       <c r="C99" t="inlineStr">
         <is>
           <t>À vista no PIX
 ou até
-1x de R$ 38,99</t>
+1x de R$ 42,34</t>
         </is>
       </c>
       <c r="D99" t="inlineStr">
         <is>
-          <t>pago</t>
+          <t>Pago</t>
+        </is>
+      </c>
+      <c r="E99" t="inlineStr">
+        <is>
+          <t>-19%</t>
         </is>
       </c>
     </row>
     <row r="100">
       <c r="A100" t="inlineStr">
         <is>
-          <t>Hub F3 Adaptador Type-c 8 em 1, para HDMI, Type-c, USB 3.0, USB 2.0, Micro SD SDe LAN - JC-TYC-860</t>
+          <t>Base com Cooler para Notebook Rise Mode, Galaxy Black X6, LED - RM-CN-06-BB</t>
         </is>
       </c>
       <c r="B100" t="inlineStr">
         <is>
-          <t>R$ 84,99</t>
+          <t>R$ 36,99</t>
         </is>
       </c>
       <c r="C100" t="inlineStr">
         <is>
           <t>À vista no PIX
 ou até
-3x de R$ 33,33</t>
+1x de R$ 39,17</t>
         </is>
       </c>
       <c r="D100" t="inlineStr">
         <is>
-          <t>pago</t>
+          <t>Pago</t>
+        </is>
+      </c>
+      <c r="E100" t="inlineStr">
+        <is>
+          <t>-25%</t>
         </is>
       </c>
     </row>
     <row r="101">
       <c r="A101" t="inlineStr">
         <is>
-          <t>Suporte de Mesa Articulado para Monitor de 17" a 27", North Bayou, Ajuste de altura com Pistão a Gás - F160NB</t>
+          <t>Pen Drive 64GB Kingston DataTraveler Exodia Onyx, USB 3.2, Preto - DTXON/64GB</t>
         </is>
       </c>
       <c r="B101" t="inlineStr">
         <is>
-          <t>R$ 249,99</t>
+          <t>R$ 38,99</t>
         </is>
       </c>
       <c r="C101" t="inlineStr">
         <is>
           <t>À vista no PIX
 ou até
-10x de R$ 26,31</t>
+1x de R$ 38,99</t>
         </is>
       </c>
       <c r="D101" t="inlineStr">
         <is>
-          <t>pago</t>
+          <t>Pago</t>
+        </is>
+      </c>
+      <c r="E101" t="inlineStr">
+        <is>
+          <t>-13%</t>
         </is>
       </c>
     </row>
     <row r="102">
       <c r="A102" t="inlineStr">
         <is>
-          <t>Cabo Fonte Sleeved Placa mãe 24p Rise Mode Aura Full White, ARGB, Branco - RM-SL-FW-ARGB</t>
+          <t>Hub F3 Adaptador Type-c 8 em 1, para HDMI, Type-c, USB 3.0, USB 2.0, Micro SD SDe LAN - JC-TYC-860</t>
         </is>
       </c>
       <c r="B102" t="inlineStr">
         <is>
-          <t>R$ 164,99</t>
+          <t>R$ 84,99</t>
         </is>
       </c>
       <c r="C102" t="inlineStr">
         <is>
           <t>À vista no PIX
 ou até
-7x de R$ 27,73</t>
+3x de R$ 33,33</t>
         </is>
       </c>
       <c r="D102" t="inlineStr">
         <is>
-          <t>pago</t>
+          <t>Pago</t>
+        </is>
+      </c>
+      <c r="E102" t="inlineStr">
+        <is>
+          <t>-26%</t>
         </is>
       </c>
     </row>
     <row r="103">
       <c r="A103" t="inlineStr">
         <is>
-          <t>Cabo Fonte Sleeved placa de video Rise Mode Aura White ARGB, 30cm, Aura 6+2p, ARGB, Branco - RM-SLV-01-FW-ARGB</t>
+          <t>Suporte de Mesa Articulado para Monitor de 17" a 27", North Bayou, Ajuste de altura com Pistão a Gás - F160NB</t>
         </is>
       </c>
       <c r="B103" t="inlineStr">
         <is>
-          <t>R$ 109,99</t>
+          <t>R$ 249,99</t>
         </is>
       </c>
       <c r="C103" t="inlineStr">
         <is>
           <t>À vista no PIX
 ou até
-5x de R$ 25,88</t>
+10x de R$ 26,31</t>
         </is>
       </c>
       <c r="D103" t="inlineStr">
         <is>
-          <t>pago</t>
+          <t>Pago</t>
+        </is>
+      </c>
+      <c r="E103" t="inlineStr">
+        <is>
+          <t>-16%</t>
         </is>
       </c>
     </row>
     <row r="104">
       <c r="A104" t="inlineStr">
         <is>
-          <t>Mesa Digitalizadora Huion Kamvas 13 com suporte ajustável, USB, Cosmo Black, Preto - GS1331</t>
+          <t>Cabo Fonte Sleeved Placa mãe 24p Rise Mode Aura Full White, ARGB, Branco - RM-SL-FW-ARGB</t>
         </is>
       </c>
       <c r="B104" t="inlineStr">
         <is>
-          <t>R$ 2.099,99</t>
+          <t>R$ 164,99</t>
         </is>
       </c>
       <c r="C104" t="inlineStr">
         <is>
           <t>À vista no PIX
 ou até
-10x de R$ 247,05</t>
+7x de R$ 27,73</t>
         </is>
       </c>
       <c r="D104" t="inlineStr">
         <is>
-          <t>pago</t>
+          <t>Pago</t>
+        </is>
+      </c>
+      <c r="E104" t="inlineStr">
+        <is>
+          <t>-13%</t>
         </is>
       </c>
     </row>
     <row r="105">
       <c r="A105" t="inlineStr">
         <is>
-          <t>Teclado Dell Kb216 - Abnt2 - Teclas Multimídia - Kb216-bk-bpor</t>
+          <t>Cabo Fonte Sleeved placa de video Rise Mode Aura White ARGB, 30cm, Aura 6+2p, ARGB, Branco - RM-SLV-01-FW-ARGB</t>
         </is>
       </c>
       <c r="B105" t="inlineStr">
         <is>
-          <t>R$ 94,05</t>
+          <t>R$ 109,99</t>
         </is>
       </c>
       <c r="C105" t="inlineStr">
         <is>
           <t>À vista no PIX
 ou até
-3x de R$ 33,00</t>
+5x de R$ 25,88</t>
         </is>
       </c>
       <c r="D105" t="inlineStr">
         <is>
-          <t>grátis</t>
+          <t>Pago</t>
+        </is>
+      </c>
+      <c r="E105" t="inlineStr">
+        <is>
+          <t>0%</t>
         </is>
       </c>
     </row>
     <row r="106">
       <c r="A106" t="inlineStr">
         <is>
-          <t>Webcam Logitech C270 HD, 720p, Microfone Integrado, USB 2.0 com 3MP - Cinza/Preta</t>
+          <t>Teclado Dell Kb216 - Abnt2 - Teclas Multimídia - Kb216-bk-bpor</t>
         </is>
       </c>
       <c r="B106" t="inlineStr">
         <is>
-          <t>R$ 184,20</t>
+          <t>R$ 94,05</t>
         </is>
       </c>
       <c r="C106" t="inlineStr">
         <is>
           <t>À vista no PIX
 ou até
-8x de R$ 25,02</t>
+3x de R$ 33,00</t>
         </is>
       </c>
       <c r="D106" t="inlineStr">
         <is>
-          <t>pago</t>
+          <t>Grátis</t>
+        </is>
+      </c>
+      <c r="E106" t="inlineStr">
+        <is>
+          <t>0%</t>
         </is>
       </c>
     </row>
     <row r="107">
       <c r="A107" t="inlineStr">
         <is>
-          <t>Webcam Intelbras Cam-1080p, Cabo USB, Full HD, Preto</t>
+          <t>Webcam Logitech C270 HD, 720p, Microfone Integrado, USB 2.0 com 3MP - Cinza/Preta</t>
         </is>
       </c>
       <c r="B107" t="inlineStr">
         <is>
-          <t>R$ 290,90</t>
+          <t>R$ 165,59</t>
         </is>
       </c>
       <c r="C107" t="inlineStr">
         <is>
           <t>À vista no PIX
 ou até
-10x de R$ 29,08</t>
+7x de R$ 25,71</t>
         </is>
       </c>
       <c r="D107" t="inlineStr">
         <is>
-          <t>grátis</t>
+          <t>Pago</t>
+        </is>
+      </c>
+      <c r="E107" t="inlineStr">
+        <is>
+          <t>0%</t>
         </is>
       </c>
     </row>
     <row r="108">
       <c r="A108" t="inlineStr">
         <is>
-          <t>Headset Profissional Monitor De Estúdio Audio-technica Ath-m20x Preto P2 E P10 Dobrável - Ath-m20x</t>
+          <t>Webcam Intelbras Cam-1080p, Cabo USB, Full HD, Preto</t>
         </is>
       </c>
       <c r="B108" t="inlineStr">
         <is>
-          <t>R$ 550,00</t>
+          <t>R$ 311,00</t>
         </is>
       </c>
       <c r="C108" t="inlineStr">
         <is>
           <t>À vista no PIX
 ou até
-10x de R$ 55,00</t>
+10x de R$ 31,10</t>
         </is>
       </c>
       <c r="D108" t="inlineStr">
         <is>
-          <t>pago</t>
+          <t>Pago</t>
+        </is>
+      </c>
+      <c r="E108" t="inlineStr">
+        <is>
+          <t>0%</t>
         </is>
       </c>
     </row>
     <row r="109">
       <c r="A109" t="inlineStr">
         <is>
-          <t>Headset Intelbras Chs 40, USB, Mono, Espuma e Microfone - 4010041</t>
+          <t>Headset Profissional Monitor De Estúdio Audio-technica Ath-m20x Preto P2 E P10 Dobrável - Ath-m20x</t>
         </is>
       </c>
       <c r="B109" t="inlineStr">
         <is>
-          <t>R$ 207,00</t>
+          <t>R$ 498,89</t>
         </is>
       </c>
       <c r="C109" t="inlineStr">
         <is>
           <t>À vista no PIX
 ou até
-8x de R$ 25,87</t>
+10x de R$ 49,88</t>
         </is>
       </c>
       <c r="D109" t="inlineStr">
         <is>
-          <t>pago</t>
+          <t>Pago</t>
+        </is>
+      </c>
+      <c r="E109" t="inlineStr">
+        <is>
+          <t>0%</t>
         </is>
       </c>
     </row>
     <row r="110">
       <c r="A110" t="inlineStr">
         <is>
-          <t>Mochila Para Notebook Lenovo, Até 15.6pol, Poliéster, 2 Compartimentos com zíper, Preto - Gx40q17225</t>
+          <t>Headset Intelbras Chs 40, USB, Mono, Espuma e Microfone - 4010041</t>
         </is>
       </c>
       <c r="B110" t="inlineStr">
         <is>
-          <t>R$ 99,00</t>
+          <t>R$ 207,00</t>
         </is>
       </c>
       <c r="C110" t="inlineStr">
         <is>
           <t>À vista no PIX
 ou até
-3x de R$ 33,00</t>
+8x de R$ 25,87</t>
         </is>
       </c>
       <c r="D110" t="inlineStr">
         <is>
-          <t>pago</t>
+          <t>Pago</t>
+        </is>
+      </c>
+      <c r="E110" t="inlineStr">
+        <is>
+          <t>0%</t>
         </is>
       </c>
     </row>
     <row r="111">
       <c r="A111" t="inlineStr">
         <is>
-          <t>Webcam Intelbras Cam HD 720p, Preto, 4290721</t>
+          <t>Mochila Para Notebook Lenovo, Até 15.6pol, Poliéster, 2 Compartimentos com zíper, Preto - Gx40q17225</t>
         </is>
       </c>
       <c r="B111" t="inlineStr">
         <is>
-          <t>R$ 176,00</t>
+          <t>R$ 99,00</t>
         </is>
       </c>
       <c r="C111" t="inlineStr">
         <is>
           <t>À vista no PIX
 ou até
-7x de R$ 25,14</t>
+3x de R$ 33,00</t>
         </is>
       </c>
       <c r="D111" t="inlineStr">
         <is>
-          <t>pago</t>
+          <t>Pago</t>
+        </is>
+      </c>
+      <c r="E111" t="inlineStr">
+        <is>
+          <t>0%</t>
         </is>
       </c>
     </row>
     <row r="112">
       <c r="A112" t="inlineStr">
         <is>
-          <t>Headset Biauricular Intelbras Usb Whs 60 Duo Preto</t>
+          <t>Webcam Intelbras Cam HD 720p, Preto, 4290721</t>
         </is>
       </c>
       <c r="B112" t="inlineStr">
         <is>
-          <t>R$ 195,90</t>
+          <t>R$ 176,00</t>
         </is>
       </c>
       <c r="C112" t="inlineStr">
         <is>
           <t>À vista no PIX
 ou até
-7x de R$ 28,55</t>
+7x de R$ 25,14</t>
         </is>
       </c>
       <c r="D112" t="inlineStr">
         <is>
-          <t>pago</t>
+          <t>Pago</t>
+        </is>
+      </c>
+      <c r="E112" t="inlineStr">
+        <is>
+          <t>0%</t>
         </is>
       </c>
     </row>
     <row r="113">
       <c r="A113" t="inlineStr">
         <is>
-          <t>Gabinete Office Pcfort E191, Mid Tower, ATX, C/ Fonte Automática 200W, USB 3.0, Preto</t>
+          <t>Headset Biauricular Intelbras Usb Whs 60 Duo Preto</t>
         </is>
       </c>
       <c r="B113" t="inlineStr">
         <is>
-          <t>R$ 223,00</t>
+          <t>R$ 195,90</t>
         </is>
       </c>
       <c r="C113" t="inlineStr">
         <is>
           <t>À vista no PIX
 ou até
-8x de R$ 27,87</t>
+7x de R$ 28,55</t>
         </is>
       </c>
       <c r="D113" t="inlineStr">
         <is>
-          <t>pago</t>
+          <t>Pago</t>
+        </is>
+      </c>
+      <c r="E113" t="inlineStr">
+        <is>
+          <t>0%</t>
         </is>
       </c>
     </row>
     <row r="114">
       <c r="A114" t="inlineStr">
         <is>
-          <t>Mouse Logitech M90, Optico, USB, Preto</t>
+          <t>Gabinete Office Pcfort E191, Mid Tower, ATX, C/ Fonte Automática 200W, USB 3.0, Preto</t>
         </is>
       </c>
       <c r="B114" t="inlineStr">
         <is>
-          <t>R$ 43,90</t>
+          <t>R$ 223,00</t>
         </is>
       </c>
       <c r="C114" t="inlineStr">
         <is>
           <t>À vista no PIX
 ou até
-1x de R$ 43,90</t>
+8x de R$ 27,87</t>
         </is>
       </c>
       <c r="D114" t="inlineStr">
         <is>
-          <t>pago</t>
+          <t>Pago</t>
+        </is>
+      </c>
+      <c r="E114" t="inlineStr">
+        <is>
+          <t>0%</t>
         </is>
       </c>
     </row>
     <row r="115">
       <c r="A115" t="inlineStr">
         <is>
-          <t>Gabinete Rack Concórdia S L-450 A, para Rack 19 com 8 baias para HDs e suporte para ATX, Micro ATX e ITX</t>
+          <t>Mouse Logitech M90, Optico, USB, Preto</t>
         </is>
       </c>
       <c r="B115" t="inlineStr">
         <is>
-          <t>R$ 423,00</t>
+          <t>R$ 43,90</t>
         </is>
       </c>
       <c r="C115" t="inlineStr">
         <is>
           <t>À vista no PIX
 ou até
-10x de R$ 42,30</t>
+1x de R$ 43,90</t>
         </is>
       </c>
       <c r="D115" t="inlineStr">
         <is>
-          <t>pago</t>
+          <t>Pago</t>
+        </is>
+      </c>
+      <c r="E115" t="inlineStr">
+        <is>
+          <t>0%</t>
         </is>
       </c>
     </row>
     <row r="116">
       <c r="A116" t="inlineStr">
         <is>
-          <t>Teclado Oex,Bluetooth Retrô Rosa, ABNT2, Tc510</t>
+          <t>Gabinete Rack Concórdia S L-450 A, para Rack 19 com 8 baias para HDs e suporte para ATX, Micro ATX e ITX</t>
         </is>
       </c>
       <c r="B116" t="inlineStr">
         <is>
-          <t>R$ 102,00</t>
+          <t>R$ 423,00</t>
         </is>
       </c>
       <c r="C116" t="inlineStr">
         <is>
           <t>À vista no PIX
 ou até
-4x de R$ 30,00</t>
+10x de R$ 42,30</t>
         </is>
       </c>
       <c r="D116" t="inlineStr">
         <is>
-          <t>grátis</t>
+          <t>Pago</t>
+        </is>
+      </c>
+      <c r="E116" t="inlineStr">
+        <is>
+          <t>0%</t>
         </is>
       </c>
     </row>
     <row r="117">
       <c r="A117" t="inlineStr">
         <is>
-          <t>Mouse Profissional Razer Deathadder V3, Ultraleve - Rz0104640100r3m</t>
+          <t>Teclado Oex,Bluetooth Retrô Rosa, ABNT2, Tc510</t>
         </is>
       </c>
       <c r="B117" t="inlineStr">
         <is>
-          <t>R$ 657,11</t>
+          <t>R$ 102,00</t>
         </is>
       </c>
       <c r="C117" t="inlineStr">
         <is>
           <t>À vista no PIX
 ou até
-10x de R$ 69,16</t>
+4x de R$ 30,00</t>
         </is>
       </c>
       <c r="D117" t="inlineStr">
         <is>
-          <t>pago</t>
+          <t>Grátis</t>
+        </is>
+      </c>
+      <c r="E117" t="inlineStr">
+        <is>
+          <t>0%</t>
         </is>
       </c>
     </row>
     <row r="118">
       <c r="A118" t="inlineStr">
         <is>
-          <t>Headset Poly C3220 USB-A/C, Profissional com Áudio de Alta Qualidade</t>
+          <t>Mouse Profissional Razer Deathadder V3, Ultraleve - Rz0104640100r3m</t>
         </is>
       </c>
       <c r="B118" t="inlineStr">
         <is>
-          <t>R$ 175,91</t>
+          <t>R$ 569,91</t>
         </is>
       </c>
       <c r="C118" t="inlineStr">
         <is>
           <t>À vista no PIX
 ou até
-7x de R$ 28,55</t>
+10x de R$ 59,99</t>
         </is>
       </c>
       <c r="D118" t="inlineStr">
         <is>
-          <t>pago</t>
+          <t>Pago</t>
+        </is>
+      </c>
+      <c r="E118" t="inlineStr">
+        <is>
+          <t>-13%</t>
         </is>
       </c>
     </row>
     <row r="119">
       <c r="A119" t="inlineStr">
         <is>
-          <t>Headset Hp Poly Blackwire C3210 Mono Usb-c+usb-a 8x214a6</t>
+          <t>Headset Poly C3220 USB-A/C, Profissional com Áudio de Alta Qualidade</t>
         </is>
       </c>
       <c r="B119" t="inlineStr">
@@ -3283,295 +3873,418 @@
       </c>
       <c r="D119" t="inlineStr">
         <is>
-          <t>pago</t>
+          <t>Pago</t>
+        </is>
+      </c>
+      <c r="E119" t="inlineStr">
+        <is>
+          <t>0%</t>
         </is>
       </c>
     </row>
     <row r="120">
       <c r="A120" t="inlineStr">
         <is>
-          <t>Videoconferência Intelbras, EVC 300, USB, HD 1080p - Preto</t>
+          <t>Headset Hp Poly Blackwire C3210 Mono Usb-c+usb-a 8x214a6</t>
         </is>
       </c>
       <c r="B120" t="inlineStr">
         <is>
-          <t>R$ 2.183,00</t>
+          <t>R$ 175,91</t>
         </is>
       </c>
       <c r="C120" t="inlineStr">
         <is>
           <t>À vista no PIX
 ou até
-10x de R$ 218,30</t>
+7x de R$ 28,55</t>
         </is>
       </c>
       <c r="D120" t="inlineStr">
         <is>
-          <t>pago</t>
+          <t>Pago</t>
+        </is>
+      </c>
+      <c r="E120" t="inlineStr">
+        <is>
+          <t>0%</t>
         </is>
       </c>
     </row>
     <row r="121">
       <c r="A121" t="inlineStr">
         <is>
-          <t>Gabinete Gamer Mymax Lion, Mid Tower, LED RGB, ATX, M-ATX e ITX, Lateral Esquerda em vidro temperado, Cooler, USB 3.0, Rosa</t>
+          <t>Videoconferência Intelbras, EVC 300, USB, HD 1080p - Preto</t>
         </is>
       </c>
       <c r="B121" t="inlineStr">
         <is>
-          <t>R$ 279,00</t>
+          <t>R$ 2.183,00</t>
         </is>
       </c>
       <c r="C121" t="inlineStr">
         <is>
           <t>À vista no PIX
 ou até
-10x de R$ 27,90</t>
+10x de R$ 218,30</t>
         </is>
       </c>
       <c r="D121" t="inlineStr">
         <is>
-          <t>pago</t>
+          <t>Pago</t>
+        </is>
+      </c>
+      <c r="E121" t="inlineStr">
+        <is>
+          <t>0%</t>
         </is>
       </c>
     </row>
     <row r="122">
       <c r="A122" t="inlineStr">
         <is>
-          <t>Gabinete Gamer Concórdia Storm X360, Mid Tower, RGB, ATX, Lateral De Vidro, Com 4 Fans RGB, Preto</t>
+          <t>Gabinete Gamer Mymax Lion, Mid Tower, LED RGB, ATX, M-ATX e ITX, Lateral Esquerda em vidro temperado, Cooler, USB 3.0, Rosa</t>
         </is>
       </c>
       <c r="B122" t="inlineStr">
         <is>
-          <t>R$ 309,00</t>
+          <t>R$ 259,37</t>
         </is>
       </c>
       <c r="C122" t="inlineStr">
         <is>
           <t>À vista no PIX
 ou até
-10x de R$ 30,90</t>
+10x de R$ 25,93</t>
         </is>
       </c>
       <c r="D122" t="inlineStr">
         <is>
-          <t>pago</t>
+          <t>Pago</t>
+        </is>
+      </c>
+      <c r="E122" t="inlineStr">
+        <is>
+          <t>-7%</t>
         </is>
       </c>
     </row>
     <row r="123">
       <c r="A123" t="inlineStr">
         <is>
-          <t>Gabinete Gamer K-mex A2g8 Infinity Streamer, Mid Tower, ArGB, ATX, Lateral Full Acrílico Transparente, C/ 3 Fans ARGB, Preto + Controle</t>
+          <t>Gabinete Gamer Concórdia Storm X360, Mid Tower, RGB, ATX, Lateral De Vidro, Com 4 Fans RGB, Preto</t>
         </is>
       </c>
       <c r="B123" t="inlineStr">
         <is>
-          <t>R$ 319,00</t>
+          <t>R$ 309,00</t>
         </is>
       </c>
       <c r="C123" t="inlineStr">
         <is>
           <t>À vista no PIX
 ou até
-10x de R$ 31,90</t>
+10x de R$ 30,90</t>
         </is>
       </c>
       <c r="D123" t="inlineStr">
         <is>
-          <t>pago</t>
+          <t>Pago</t>
+        </is>
+      </c>
+      <c r="E123" t="inlineStr">
+        <is>
+          <t>0%</t>
         </is>
       </c>
     </row>
     <row r="124">
       <c r="A124" t="inlineStr">
         <is>
-          <t>Gabinete Gamer Pcfort Lines, Mid Tower, RGB, ATX, Lateral De Vidro, C/ 3 Fans, Preto</t>
+          <t>Gabinete Gamer K-mex A2g8 Infinity Streamer, Mid Tower, ArGB, ATX, Lateral Full Acrílico Transparente, C/ 3 Fans ARGB, Preto + Controle</t>
         </is>
       </c>
       <c r="B124" t="inlineStr">
         <is>
-          <t>R$ 238,00</t>
+          <t>R$ 319,00</t>
         </is>
       </c>
       <c r="C124" t="inlineStr">
         <is>
           <t>À vista no PIX
 ou até
-9x de R$ 26,44</t>
+10x de R$ 31,90</t>
         </is>
       </c>
       <c r="D124" t="inlineStr">
         <is>
-          <t>pago</t>
+          <t>Pago</t>
+        </is>
+      </c>
+      <c r="E124" t="inlineStr">
+        <is>
+          <t>0%</t>
         </is>
       </c>
     </row>
     <row r="125">
       <c r="A125" t="inlineStr">
         <is>
-          <t>Gabinete Gamer Draxen Ithnan, Mid Tower, ArGB, Vidro Temperado - Preto</t>
+          <t>Gabinete Gamer Pcfort Lines, Mid Tower, RGB, ATX, Lateral De Vidro, C/ 3 Fans, Preto</t>
         </is>
       </c>
       <c r="B125" t="inlineStr">
         <is>
-          <t>R$ 239,00</t>
+          <t>R$ 238,00</t>
         </is>
       </c>
       <c r="C125" t="inlineStr">
         <is>
           <t>À vista no PIX
 ou até
-9x de R$ 26,55</t>
+9x de R$ 26,44</t>
         </is>
       </c>
       <c r="D125" t="inlineStr">
         <is>
-          <t>pago</t>
+          <t>Pago</t>
+        </is>
+      </c>
+      <c r="E125" t="inlineStr">
+        <is>
+          <t>0%</t>
         </is>
       </c>
     </row>
     <row r="126">
       <c r="A126" t="inlineStr">
         <is>
-          <t>Gabinete Gamer Concórdia Creative, Mid Tower, ARGB, Vidro Frontal Para Escrita, 3 Fans</t>
+          <t>Gabinete Gamer Draxen Ithnan, Mid Tower, ArGB, Vidro Temperado - Preto</t>
         </is>
       </c>
       <c r="B126" t="inlineStr">
         <is>
-          <t>R$ 299,00</t>
+          <t>R$ 239,00</t>
         </is>
       </c>
       <c r="C126" t="inlineStr">
         <is>
           <t>À vista no PIX
 ou até
-10x de R$ 29,90</t>
+9x de R$ 26,55</t>
         </is>
       </c>
       <c r="D126" t="inlineStr">
         <is>
-          <t>pago</t>
+          <t>Pago</t>
+        </is>
+      </c>
+      <c r="E126" t="inlineStr">
+        <is>
+          <t>0%</t>
         </is>
       </c>
     </row>
     <row r="127">
       <c r="A127" t="inlineStr">
         <is>
-          <t>Gabinete Gamer Arbaton Vidro Temperado ARGB Branco Draxen(drn30a-wh)</t>
+          <t>Gabinete Gamer Concórdia Creative, Mid Tower, ARGB, Vidro Frontal Para Escrita, 3 Fans</t>
         </is>
       </c>
       <c r="B127" t="inlineStr">
         <is>
-          <t>R$ 549,90</t>
+          <t>R$ 299,00</t>
         </is>
       </c>
       <c r="C127" t="inlineStr">
         <is>
           <t>À vista no PIX
 ou até
-10x de R$ 54,98</t>
+10x de R$ 29,90</t>
         </is>
       </c>
       <c r="D127" t="inlineStr">
         <is>
-          <t>pago</t>
+          <t>Pago</t>
+        </is>
+      </c>
+      <c r="E127" t="inlineStr">
+        <is>
+          <t>0%</t>
         </is>
       </c>
     </row>
     <row r="128">
       <c r="A128" t="inlineStr">
         <is>
-          <t>Mesa Digitalizadora Huion Kamvas Plus 22", Tela Full HD, Caneta PenTech 3.0, 8192 Níveis de Pressão, com Luva de Desenho, Preto - GS2202</t>
+          <t>Gabinete Gamer Arbaton Vidro Temperado ARGB Preto Draxen(drn30a-bk).</t>
         </is>
       </c>
       <c r="B128" t="inlineStr">
         <is>
-          <t>R$ 3.599,99</t>
+          <t>R$ 499,90</t>
         </is>
       </c>
       <c r="C128" t="inlineStr">
         <is>
           <t>À vista no PIX
 ou até
-10x de R$ 423,52</t>
+10x de R$ 49,98</t>
         </is>
       </c>
       <c r="D128" t="inlineStr">
         <is>
-          <t>pago</t>
+          <t>Pago</t>
+        </is>
+      </c>
+      <c r="E128" t="inlineStr">
+        <is>
+          <t>0%</t>
         </is>
       </c>
     </row>
     <row r="129">
       <c r="A129" t="inlineStr">
         <is>
-          <t>Suporte Ergonômico Multiarticulado de Mesa para Monitor 17 a 35 ELG F98HDMI, Pistão à Gás, VESA, Grafite - F98HDMI</t>
+          <t>Gabinete Gamer Arbaton Vidro Temperado ARGB Branco Draxen(drn30a-wh)</t>
         </is>
       </c>
       <c r="B129" t="inlineStr">
         <is>
-          <t>R$ 189,99</t>
+          <t>R$ 511,20</t>
         </is>
       </c>
       <c r="C129" t="inlineStr">
         <is>
           <t>À vista no PIX
 ou até
-8x de R$ 27,94</t>
+10x de R$ 51,12</t>
         </is>
       </c>
       <c r="D129" t="inlineStr">
         <is>
-          <t>pago</t>
+          <t>Pago</t>
+        </is>
+      </c>
+      <c r="E129" t="inlineStr">
+        <is>
+          <t>-7%</t>
         </is>
       </c>
     </row>
     <row r="130">
       <c r="A130" t="inlineStr">
         <is>
-          <t>Suporte de Mesa Articulado para Monitor de 17" a 30", North Bayou, Ajuste de altura com Pistão a Gás - F80 NB</t>
+          <t>Mesa Digitalizadora Huion Kamvas Plus 22", Tela Full HD, Caneta PenTech 3.0, 8192 Níveis de Pressão, com Luva de Desenho, Preto - GS2202</t>
         </is>
       </c>
       <c r="B130" t="inlineStr">
         <is>
-          <t>R$ 149,99</t>
+          <t>R$ 3.599,99</t>
         </is>
       </c>
       <c r="C130" t="inlineStr">
         <is>
           <t>À vista no PIX
 ou até
-7x de R$ 25,20</t>
+10x de R$ 423,52</t>
         </is>
       </c>
       <c r="D130" t="inlineStr">
         <is>
-          <t>pago</t>
+          <t>Pago</t>
+        </is>
+      </c>
+      <c r="E130" t="inlineStr">
+        <is>
+          <t>-4%</t>
         </is>
       </c>
     </row>
     <row r="131">
       <c r="A131" t="inlineStr">
         <is>
+          <t>Suporte Ergonômico Multiarticulado de Mesa para Monitor 17 a 35 ELG F98HDMI, Pistão à Gás, VESA, Grafite - F98HDMI</t>
+        </is>
+      </c>
+      <c r="B131" t="inlineStr">
+        <is>
+          <t>R$ 189,99</t>
+        </is>
+      </c>
+      <c r="C131" t="inlineStr">
+        <is>
+          <t>À vista no PIX
+ou até
+8x de R$ 27,94</t>
+        </is>
+      </c>
+      <c r="D131" t="inlineStr">
+        <is>
+          <t>Pago</t>
+        </is>
+      </c>
+      <c r="E131" t="inlineStr">
+        <is>
+          <t>-24%</t>
+        </is>
+      </c>
+    </row>
+    <row r="132">
+      <c r="A132" t="inlineStr">
+        <is>
+          <t>Suporte de Mesa Articulado para Monitor de 17" a 30", North Bayou, Ajuste de altura com Pistão a Gás - F80 NB</t>
+        </is>
+      </c>
+      <c r="B132" t="inlineStr">
+        <is>
+          <t>R$ 149,99</t>
+        </is>
+      </c>
+      <c r="C132" t="inlineStr">
+        <is>
+          <t>À vista no PIX
+ou até
+7x de R$ 25,20</t>
+        </is>
+      </c>
+      <c r="D132" t="inlineStr">
+        <is>
+          <t>Pago</t>
+        </is>
+      </c>
+      <c r="E132" t="inlineStr">
+        <is>
+          <t>-25%</t>
+        </is>
+      </c>
+    </row>
+    <row r="133">
+      <c r="A133" t="inlineStr">
+        <is>
           <t>Suporte Articulado de Mesa para 2 Monitores DE 17" a 35"+ ELG, Com Pistão a Gás, 2 Cabos HDMI de 2.5m - F196HDMI</t>
         </is>
       </c>
-      <c r="B131" t="inlineStr">
+      <c r="B133" t="inlineStr">
         <is>
           <t>R$ 399,99</t>
         </is>
       </c>
-      <c r="C131" t="inlineStr">
+      <c r="C133" t="inlineStr">
         <is>
           <t>À vista no PIX
 ou até
 10x de R$ 47,05</t>
         </is>
       </c>
-      <c r="D131" t="inlineStr">
-        <is>
-          <t>pago</t>
+      <c r="D133" t="inlineStr">
+        <is>
+          <t>Pago</t>
+        </is>
+      </c>
+      <c r="E133" t="inlineStr">
+        <is>
+          <t>-19%</t>
         </is>
       </c>
     </row>

</xml_diff>